<commit_message>
Added Let and some more tests
</commit_message>
<xml_diff>
--- a/Instruction Set.xlsx
+++ b/Instruction Set.xlsx
@@ -1309,9 +1309,114 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1321,143 +1426,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4702,8 +4702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL121" sqref="AL121"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4892,16 +4892,16 @@
       <c r="AI2" s="5">
         <v>-1</v>
       </c>
-      <c r="AJ2" s="96" t="s">
+      <c r="AJ2" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="110"/>
-      <c r="AL2" s="110"/>
-      <c r="AM2" s="110"/>
-      <c r="AN2" s="110"/>
-      <c r="AO2" s="110"/>
-      <c r="AP2" s="110"/>
-      <c r="AQ2" s="110"/>
+      <c r="AK2" s="103"/>
+      <c r="AL2" s="103"/>
+      <c r="AM2" s="103"/>
+      <c r="AN2" s="103"/>
+      <c r="AO2" s="103"/>
+      <c r="AP2" s="103"/>
+      <c r="AQ2" s="103"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
@@ -4947,16 +4947,16 @@
       <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
       <c r="AI3" s="8"/>
-      <c r="AJ3" s="96" t="s">
+      <c r="AJ3" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="110"/>
-      <c r="AO3" s="110"/>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
+      <c r="AK3" s="103"/>
+      <c r="AL3" s="103"/>
+      <c r="AM3" s="103"/>
+      <c r="AN3" s="103"/>
+      <c r="AO3" s="103"/>
+      <c r="AP3" s="103"/>
+      <c r="AQ3" s="103"/>
     </row>
     <row r="4" spans="1:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
@@ -5008,16 +5008,16 @@
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
       <c r="AI4" s="11"/>
-      <c r="AJ4" s="96" t="s">
+      <c r="AJ4" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="AK4" s="110"/>
-      <c r="AL4" s="110"/>
-      <c r="AM4" s="110"/>
-      <c r="AN4" s="110"/>
-      <c r="AO4" s="110"/>
-      <c r="AP4" s="110"/>
-      <c r="AQ4" s="110"/>
+      <c r="AK4" s="103"/>
+      <c r="AL4" s="103"/>
+      <c r="AM4" s="103"/>
+      <c r="AN4" s="103"/>
+      <c r="AO4" s="103"/>
+      <c r="AP4" s="103"/>
+      <c r="AQ4" s="103"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
@@ -5057,16 +5057,16 @@
       <c r="AG5" s="13"/>
       <c r="AH5" s="13"/>
       <c r="AI5" s="13"/>
-      <c r="AJ5" s="111" t="s">
+      <c r="AJ5" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="AK5" s="112"/>
-      <c r="AL5" s="112"/>
-      <c r="AM5" s="112"/>
-      <c r="AN5" s="112"/>
-      <c r="AO5" s="112"/>
-      <c r="AP5" s="112"/>
-      <c r="AQ5" s="112"/>
+      <c r="AK5" s="109"/>
+      <c r="AL5" s="109"/>
+      <c r="AM5" s="109"/>
+      <c r="AN5" s="109"/>
+      <c r="AO5" s="109"/>
+      <c r="AP5" s="109"/>
+      <c r="AQ5" s="109"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
@@ -5108,16 +5108,16 @@
       <c r="AG6" s="8"/>
       <c r="AH6" s="8"/>
       <c r="AI6" s="8"/>
-      <c r="AJ6" s="96" t="s">
+      <c r="AJ6" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="AK6" s="97"/>
-      <c r="AL6" s="97"/>
-      <c r="AM6" s="97"/>
-      <c r="AN6" s="97"/>
-      <c r="AO6" s="97"/>
-      <c r="AP6" s="97"/>
-      <c r="AQ6" s="97"/>
+      <c r="AK6" s="106"/>
+      <c r="AL6" s="106"/>
+      <c r="AM6" s="106"/>
+      <c r="AN6" s="106"/>
+      <c r="AO6" s="106"/>
+      <c r="AP6" s="106"/>
+      <c r="AQ6" s="106"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
@@ -5163,16 +5163,16 @@
       <c r="AG7" s="8"/>
       <c r="AH7" s="8"/>
       <c r="AI7" s="8"/>
-      <c r="AJ7" s="96" t="s">
+      <c r="AJ7" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="AK7" s="97"/>
-      <c r="AL7" s="97"/>
-      <c r="AM7" s="97"/>
-      <c r="AN7" s="97"/>
-      <c r="AO7" s="97"/>
-      <c r="AP7" s="97"/>
-      <c r="AQ7" s="97"/>
+      <c r="AK7" s="106"/>
+      <c r="AL7" s="106"/>
+      <c r="AM7" s="106"/>
+      <c r="AN7" s="106"/>
+      <c r="AO7" s="106"/>
+      <c r="AP7" s="106"/>
+      <c r="AQ7" s="106"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
@@ -5218,16 +5218,16 @@
       <c r="AG8" s="8"/>
       <c r="AH8" s="8"/>
       <c r="AI8" s="8"/>
-      <c r="AJ8" s="96" t="s">
+      <c r="AJ8" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="AK8" s="97"/>
-      <c r="AL8" s="97"/>
-      <c r="AM8" s="97"/>
-      <c r="AN8" s="97"/>
-      <c r="AO8" s="97"/>
-      <c r="AP8" s="97"/>
-      <c r="AQ8" s="97"/>
+      <c r="AK8" s="106"/>
+      <c r="AL8" s="106"/>
+      <c r="AM8" s="106"/>
+      <c r="AN8" s="106"/>
+      <c r="AO8" s="106"/>
+      <c r="AP8" s="106"/>
+      <c r="AQ8" s="106"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
@@ -5269,16 +5269,16 @@
       <c r="AG9" s="8"/>
       <c r="AH9" s="8"/>
       <c r="AI9" s="8"/>
-      <c r="AJ9" s="96" t="s">
+      <c r="AJ9" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="AK9" s="97"/>
-      <c r="AL9" s="97"/>
-      <c r="AM9" s="97"/>
-      <c r="AN9" s="97"/>
-      <c r="AO9" s="97"/>
-      <c r="AP9" s="97"/>
-      <c r="AQ9" s="97"/>
+      <c r="AK9" s="106"/>
+      <c r="AL9" s="106"/>
+      <c r="AM9" s="106"/>
+      <c r="AN9" s="106"/>
+      <c r="AO9" s="106"/>
+      <c r="AP9" s="106"/>
+      <c r="AQ9" s="106"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
@@ -5320,16 +5320,16 @@
       <c r="AG10" s="8"/>
       <c r="AH10" s="8"/>
       <c r="AI10" s="8"/>
-      <c r="AJ10" s="96" t="s">
+      <c r="AJ10" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="AK10" s="97"/>
-      <c r="AL10" s="97"/>
-      <c r="AM10" s="97"/>
-      <c r="AN10" s="97"/>
-      <c r="AO10" s="97"/>
-      <c r="AP10" s="97"/>
-      <c r="AQ10" s="97"/>
+      <c r="AK10" s="106"/>
+      <c r="AL10" s="106"/>
+      <c r="AM10" s="106"/>
+      <c r="AN10" s="106"/>
+      <c r="AO10" s="106"/>
+      <c r="AP10" s="106"/>
+      <c r="AQ10" s="106"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
@@ -5371,16 +5371,16 @@
       <c r="AG11" s="8"/>
       <c r="AH11" s="8"/>
       <c r="AI11" s="8"/>
-      <c r="AJ11" s="96" t="s">
+      <c r="AJ11" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="AK11" s="97"/>
-      <c r="AL11" s="97"/>
-      <c r="AM11" s="97"/>
-      <c r="AN11" s="97"/>
-      <c r="AO11" s="97"/>
-      <c r="AP11" s="97"/>
-      <c r="AQ11" s="97"/>
+      <c r="AK11" s="106"/>
+      <c r="AL11" s="106"/>
+      <c r="AM11" s="106"/>
+      <c r="AN11" s="106"/>
+      <c r="AO11" s="106"/>
+      <c r="AP11" s="106"/>
+      <c r="AQ11" s="106"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
@@ -5422,16 +5422,16 @@
       <c r="AG12" s="8"/>
       <c r="AH12" s="8"/>
       <c r="AI12" s="8"/>
-      <c r="AJ12" s="96" t="s">
+      <c r="AJ12" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="AK12" s="97"/>
-      <c r="AL12" s="97"/>
-      <c r="AM12" s="97"/>
-      <c r="AN12" s="97"/>
-      <c r="AO12" s="97"/>
-      <c r="AP12" s="97"/>
-      <c r="AQ12" s="97"/>
+      <c r="AK12" s="106"/>
+      <c r="AL12" s="106"/>
+      <c r="AM12" s="106"/>
+      <c r="AN12" s="106"/>
+      <c r="AO12" s="106"/>
+      <c r="AP12" s="106"/>
+      <c r="AQ12" s="106"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
@@ -5473,16 +5473,16 @@
       <c r="AG13" s="8"/>
       <c r="AH13" s="8"/>
       <c r="AI13" s="8"/>
-      <c r="AJ13" s="96" t="s">
+      <c r="AJ13" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="AK13" s="97"/>
-      <c r="AL13" s="97"/>
-      <c r="AM13" s="97"/>
-      <c r="AN13" s="97"/>
-      <c r="AO13" s="97"/>
-      <c r="AP13" s="97"/>
-      <c r="AQ13" s="97"/>
+      <c r="AK13" s="106"/>
+      <c r="AL13" s="106"/>
+      <c r="AM13" s="106"/>
+      <c r="AN13" s="106"/>
+      <c r="AO13" s="106"/>
+      <c r="AP13" s="106"/>
+      <c r="AQ13" s="106"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
@@ -5524,14 +5524,14 @@
       <c r="AG14" s="8"/>
       <c r="AH14" s="8"/>
       <c r="AI14" s="8"/>
-      <c r="AJ14" s="96"/>
-      <c r="AK14" s="97"/>
-      <c r="AL14" s="97"/>
-      <c r="AM14" s="97"/>
-      <c r="AN14" s="97"/>
-      <c r="AO14" s="97"/>
-      <c r="AP14" s="97"/>
-      <c r="AQ14" s="97"/>
+      <c r="AJ14" s="102"/>
+      <c r="AK14" s="106"/>
+      <c r="AL14" s="106"/>
+      <c r="AM14" s="106"/>
+      <c r="AN14" s="106"/>
+      <c r="AO14" s="106"/>
+      <c r="AP14" s="106"/>
+      <c r="AQ14" s="106"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
@@ -5575,16 +5575,16 @@
       <c r="AG15" s="8"/>
       <c r="AH15" s="8"/>
       <c r="AI15" s="8"/>
-      <c r="AJ15" s="96" t="s">
+      <c r="AJ15" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="AK15" s="97"/>
-      <c r="AL15" s="97"/>
-      <c r="AM15" s="97"/>
-      <c r="AN15" s="97"/>
-      <c r="AO15" s="97"/>
-      <c r="AP15" s="97"/>
-      <c r="AQ15" s="97"/>
+      <c r="AK15" s="106"/>
+      <c r="AL15" s="106"/>
+      <c r="AM15" s="106"/>
+      <c r="AN15" s="106"/>
+      <c r="AO15" s="106"/>
+      <c r="AP15" s="106"/>
+      <c r="AQ15" s="106"/>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
@@ -5628,16 +5628,16 @@
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
       <c r="AI16" s="8"/>
-      <c r="AJ16" s="96" t="s">
+      <c r="AJ16" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="AK16" s="97"/>
-      <c r="AL16" s="97"/>
-      <c r="AM16" s="97"/>
-      <c r="AN16" s="97"/>
-      <c r="AO16" s="97"/>
-      <c r="AP16" s="97"/>
-      <c r="AQ16" s="97"/>
+      <c r="AK16" s="106"/>
+      <c r="AL16" s="106"/>
+      <c r="AM16" s="106"/>
+      <c r="AN16" s="106"/>
+      <c r="AO16" s="106"/>
+      <c r="AP16" s="106"/>
+      <c r="AQ16" s="106"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
@@ -5681,16 +5681,16 @@
       <c r="AG17" s="8"/>
       <c r="AH17" s="8"/>
       <c r="AI17" s="8"/>
-      <c r="AJ17" s="96" t="s">
+      <c r="AJ17" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="AK17" s="97"/>
-      <c r="AL17" s="97"/>
-      <c r="AM17" s="97"/>
-      <c r="AN17" s="97"/>
-      <c r="AO17" s="97"/>
-      <c r="AP17" s="97"/>
-      <c r="AQ17" s="97"/>
+      <c r="AK17" s="106"/>
+      <c r="AL17" s="106"/>
+      <c r="AM17" s="106"/>
+      <c r="AN17" s="106"/>
+      <c r="AO17" s="106"/>
+      <c r="AP17" s="106"/>
+      <c r="AQ17" s="106"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
@@ -5734,16 +5734,16 @@
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
       <c r="AI18" s="8"/>
-      <c r="AJ18" s="96" t="s">
+      <c r="AJ18" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="AK18" s="97"/>
-      <c r="AL18" s="97"/>
-      <c r="AM18" s="97"/>
-      <c r="AN18" s="97"/>
-      <c r="AO18" s="97"/>
-      <c r="AP18" s="97"/>
-      <c r="AQ18" s="97"/>
+      <c r="AK18" s="106"/>
+      <c r="AL18" s="106"/>
+      <c r="AM18" s="106"/>
+      <c r="AN18" s="106"/>
+      <c r="AO18" s="106"/>
+      <c r="AP18" s="106"/>
+      <c r="AQ18" s="106"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
@@ -5785,16 +5785,16 @@
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
       <c r="AI19" s="8"/>
-      <c r="AJ19" s="96" t="s">
+      <c r="AJ19" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="AK19" s="97"/>
-      <c r="AL19" s="97"/>
-      <c r="AM19" s="97"/>
-      <c r="AN19" s="97"/>
-      <c r="AO19" s="97"/>
-      <c r="AP19" s="97"/>
-      <c r="AQ19" s="97"/>
+      <c r="AK19" s="106"/>
+      <c r="AL19" s="106"/>
+      <c r="AM19" s="106"/>
+      <c r="AN19" s="106"/>
+      <c r="AO19" s="106"/>
+      <c r="AP19" s="106"/>
+      <c r="AQ19" s="106"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
@@ -5842,16 +5842,16 @@
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
       <c r="AI20" s="8"/>
-      <c r="AJ20" s="96" t="s">
+      <c r="AJ20" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="AK20" s="97"/>
-      <c r="AL20" s="97"/>
-      <c r="AM20" s="97"/>
-      <c r="AN20" s="97"/>
-      <c r="AO20" s="97"/>
-      <c r="AP20" s="97"/>
-      <c r="AQ20" s="97"/>
+      <c r="AK20" s="106"/>
+      <c r="AL20" s="106"/>
+      <c r="AM20" s="106"/>
+      <c r="AN20" s="106"/>
+      <c r="AO20" s="106"/>
+      <c r="AP20" s="106"/>
+      <c r="AQ20" s="106"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
@@ -5895,16 +5895,16 @@
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
-      <c r="AJ21" s="96" t="s">
+      <c r="AJ21" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="AK21" s="97"/>
-      <c r="AL21" s="97"/>
-      <c r="AM21" s="97"/>
-      <c r="AN21" s="97"/>
-      <c r="AO21" s="97"/>
-      <c r="AP21" s="97"/>
-      <c r="AQ21" s="97"/>
+      <c r="AK21" s="106"/>
+      <c r="AL21" s="106"/>
+      <c r="AM21" s="106"/>
+      <c r="AN21" s="106"/>
+      <c r="AO21" s="106"/>
+      <c r="AP21" s="106"/>
+      <c r="AQ21" s="106"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
@@ -5946,16 +5946,16 @@
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
       <c r="AI22" s="8"/>
-      <c r="AJ22" s="96" t="s">
+      <c r="AJ22" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="AK22" s="97"/>
-      <c r="AL22" s="97"/>
-      <c r="AM22" s="97"/>
-      <c r="AN22" s="97"/>
-      <c r="AO22" s="97"/>
-      <c r="AP22" s="97"/>
-      <c r="AQ22" s="97"/>
+      <c r="AK22" s="106"/>
+      <c r="AL22" s="106"/>
+      <c r="AM22" s="106"/>
+      <c r="AN22" s="106"/>
+      <c r="AO22" s="106"/>
+      <c r="AP22" s="106"/>
+      <c r="AQ22" s="106"/>
     </row>
     <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="27" spans="1:43" ht="30.4" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6132,16 +6132,16 @@
       <c r="AI28" s="5">
         <v>-1</v>
       </c>
-      <c r="AJ28" s="96" t="s">
+      <c r="AJ28" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="AK28" s="110"/>
-      <c r="AL28" s="110"/>
-      <c r="AM28" s="110"/>
-      <c r="AN28" s="110"/>
-      <c r="AO28" s="110"/>
-      <c r="AP28" s="110"/>
-      <c r="AQ28" s="110"/>
+      <c r="AK28" s="103"/>
+      <c r="AL28" s="103"/>
+      <c r="AM28" s="103"/>
+      <c r="AN28" s="103"/>
+      <c r="AO28" s="103"/>
+      <c r="AP28" s="103"/>
+      <c r="AQ28" s="103"/>
     </row>
     <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
@@ -6187,16 +6187,16 @@
       <c r="AG29" s="8"/>
       <c r="AH29" s="8"/>
       <c r="AI29" s="8"/>
-      <c r="AJ29" s="96" t="s">
+      <c r="AJ29" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="AK29" s="110"/>
-      <c r="AL29" s="110"/>
-      <c r="AM29" s="110"/>
-      <c r="AN29" s="110"/>
-      <c r="AO29" s="110"/>
-      <c r="AP29" s="110"/>
-      <c r="AQ29" s="110"/>
+      <c r="AK29" s="103"/>
+      <c r="AL29" s="103"/>
+      <c r="AM29" s="103"/>
+      <c r="AN29" s="103"/>
+      <c r="AO29" s="103"/>
+      <c r="AP29" s="103"/>
+      <c r="AQ29" s="103"/>
     </row>
     <row r="30" spans="1:43" ht="14.65" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="10" t="s">
@@ -6248,16 +6248,16 @@
       <c r="AG30" s="11"/>
       <c r="AH30" s="11"/>
       <c r="AI30" s="11"/>
-      <c r="AJ30" s="96" t="s">
+      <c r="AJ30" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="AK30" s="110"/>
-      <c r="AL30" s="110"/>
-      <c r="AM30" s="110"/>
-      <c r="AN30" s="110"/>
-      <c r="AO30" s="110"/>
-      <c r="AP30" s="110"/>
-      <c r="AQ30" s="110"/>
+      <c r="AK30" s="103"/>
+      <c r="AL30" s="103"/>
+      <c r="AM30" s="103"/>
+      <c r="AN30" s="103"/>
+      <c r="AO30" s="103"/>
+      <c r="AP30" s="103"/>
+      <c r="AQ30" s="103"/>
     </row>
     <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
@@ -6299,16 +6299,16 @@
       <c r="AG31" s="14"/>
       <c r="AH31" s="14"/>
       <c r="AI31" s="14"/>
-      <c r="AJ31" s="96" t="s">
+      <c r="AJ31" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="AK31" s="97"/>
-      <c r="AL31" s="97"/>
-      <c r="AM31" s="97"/>
-      <c r="AN31" s="97"/>
-      <c r="AO31" s="97"/>
-      <c r="AP31" s="97"/>
-      <c r="AQ31" s="97"/>
+      <c r="AK31" s="106"/>
+      <c r="AL31" s="106"/>
+      <c r="AM31" s="106"/>
+      <c r="AN31" s="106"/>
+      <c r="AO31" s="106"/>
+      <c r="AP31" s="106"/>
+      <c r="AQ31" s="106"/>
     </row>
     <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
@@ -6354,16 +6354,16 @@
       <c r="AG32" s="8"/>
       <c r="AH32" s="8"/>
       <c r="AI32" s="8"/>
-      <c r="AJ32" s="96" t="s">
+      <c r="AJ32" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="AK32" s="110"/>
-      <c r="AL32" s="110"/>
-      <c r="AM32" s="110"/>
-      <c r="AN32" s="110"/>
-      <c r="AO32" s="110"/>
-      <c r="AP32" s="110"/>
-      <c r="AQ32" s="110"/>
+      <c r="AK32" s="103"/>
+      <c r="AL32" s="103"/>
+      <c r="AM32" s="103"/>
+      <c r="AN32" s="103"/>
+      <c r="AO32" s="103"/>
+      <c r="AP32" s="103"/>
+      <c r="AQ32" s="103"/>
     </row>
     <row r="33" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
@@ -6405,16 +6405,16 @@
       <c r="AG33" s="8"/>
       <c r="AH33" s="8"/>
       <c r="AI33" s="8"/>
-      <c r="AJ33" s="96" t="s">
+      <c r="AJ33" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="AK33" s="110"/>
-      <c r="AL33" s="110"/>
-      <c r="AM33" s="110"/>
-      <c r="AN33" s="110"/>
-      <c r="AO33" s="110"/>
-      <c r="AP33" s="110"/>
-      <c r="AQ33" s="110"/>
+      <c r="AK33" s="103"/>
+      <c r="AL33" s="103"/>
+      <c r="AM33" s="103"/>
+      <c r="AN33" s="103"/>
+      <c r="AO33" s="103"/>
+      <c r="AP33" s="103"/>
+      <c r="AQ33" s="103"/>
     </row>
     <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
@@ -6456,16 +6456,16 @@
       <c r="AG34" s="8"/>
       <c r="AH34" s="8"/>
       <c r="AI34" s="8"/>
-      <c r="AJ34" s="96" t="s">
+      <c r="AJ34" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="AK34" s="110"/>
-      <c r="AL34" s="110"/>
-      <c r="AM34" s="110"/>
-      <c r="AN34" s="110"/>
-      <c r="AO34" s="110"/>
-      <c r="AP34" s="110"/>
-      <c r="AQ34" s="110"/>
+      <c r="AK34" s="103"/>
+      <c r="AL34" s="103"/>
+      <c r="AM34" s="103"/>
+      <c r="AN34" s="103"/>
+      <c r="AO34" s="103"/>
+      <c r="AP34" s="103"/>
+      <c r="AQ34" s="103"/>
     </row>
     <row r="35" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
@@ -6507,16 +6507,16 @@
       <c r="AG35" s="8"/>
       <c r="AH35" s="8"/>
       <c r="AI35" s="8"/>
-      <c r="AJ35" s="96" t="s">
+      <c r="AJ35" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="AK35" s="110"/>
-      <c r="AL35" s="110"/>
-      <c r="AM35" s="110"/>
-      <c r="AN35" s="110"/>
-      <c r="AO35" s="110"/>
-      <c r="AP35" s="110"/>
-      <c r="AQ35" s="110"/>
+      <c r="AK35" s="103"/>
+      <c r="AL35" s="103"/>
+      <c r="AM35" s="103"/>
+      <c r="AN35" s="103"/>
+      <c r="AO35" s="103"/>
+      <c r="AP35" s="103"/>
+      <c r="AQ35" s="103"/>
     </row>
     <row r="36" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
@@ -6558,16 +6558,16 @@
       <c r="AG36" s="17"/>
       <c r="AH36" s="17"/>
       <c r="AI36" s="17"/>
-      <c r="AJ36" s="113" t="s">
+      <c r="AJ36" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="AK36" s="114"/>
-      <c r="AL36" s="114"/>
-      <c r="AM36" s="114"/>
-      <c r="AN36" s="114"/>
-      <c r="AO36" s="114"/>
-      <c r="AP36" s="114"/>
-      <c r="AQ36" s="114"/>
+      <c r="AK36" s="105"/>
+      <c r="AL36" s="105"/>
+      <c r="AM36" s="105"/>
+      <c r="AN36" s="105"/>
+      <c r="AO36" s="105"/>
+      <c r="AP36" s="105"/>
+      <c r="AQ36" s="105"/>
     </row>
     <row r="37" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
@@ -6609,14 +6609,14 @@
       <c r="AG37" s="8"/>
       <c r="AH37" s="8"/>
       <c r="AI37" s="8"/>
-      <c r="AJ37" s="96"/>
-      <c r="AK37" s="110"/>
-      <c r="AL37" s="110"/>
-      <c r="AM37" s="110"/>
-      <c r="AN37" s="110"/>
-      <c r="AO37" s="110"/>
-      <c r="AP37" s="110"/>
-      <c r="AQ37" s="110"/>
+      <c r="AJ37" s="102"/>
+      <c r="AK37" s="103"/>
+      <c r="AL37" s="103"/>
+      <c r="AM37" s="103"/>
+      <c r="AN37" s="103"/>
+      <c r="AO37" s="103"/>
+      <c r="AP37" s="103"/>
+      <c r="AQ37" s="103"/>
     </row>
     <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
@@ -6660,16 +6660,16 @@
       <c r="AG38" s="8"/>
       <c r="AH38" s="8"/>
       <c r="AI38" s="8"/>
-      <c r="AJ38" s="96" t="s">
+      <c r="AJ38" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="AK38" s="110"/>
-      <c r="AL38" s="110"/>
-      <c r="AM38" s="110"/>
-      <c r="AN38" s="110"/>
-      <c r="AO38" s="110"/>
-      <c r="AP38" s="110"/>
-      <c r="AQ38" s="110"/>
+      <c r="AK38" s="103"/>
+      <c r="AL38" s="103"/>
+      <c r="AM38" s="103"/>
+      <c r="AN38" s="103"/>
+      <c r="AO38" s="103"/>
+      <c r="AP38" s="103"/>
+      <c r="AQ38" s="103"/>
     </row>
     <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
@@ -6713,16 +6713,16 @@
       <c r="AG39" s="8"/>
       <c r="AH39" s="8"/>
       <c r="AI39" s="8"/>
-      <c r="AJ39" s="96" t="s">
+      <c r="AJ39" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="AK39" s="110"/>
-      <c r="AL39" s="110"/>
-      <c r="AM39" s="110"/>
-      <c r="AN39" s="110"/>
-      <c r="AO39" s="110"/>
-      <c r="AP39" s="110"/>
-      <c r="AQ39" s="110"/>
+      <c r="AK39" s="103"/>
+      <c r="AL39" s="103"/>
+      <c r="AM39" s="103"/>
+      <c r="AN39" s="103"/>
+      <c r="AO39" s="103"/>
+      <c r="AP39" s="103"/>
+      <c r="AQ39" s="103"/>
     </row>
     <row r="40" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
@@ -6766,16 +6766,16 @@
       <c r="AG40" s="8"/>
       <c r="AH40" s="8"/>
       <c r="AI40" s="8"/>
-      <c r="AJ40" s="96" t="s">
+      <c r="AJ40" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="AK40" s="110"/>
-      <c r="AL40" s="110"/>
-      <c r="AM40" s="110"/>
-      <c r="AN40" s="110"/>
-      <c r="AO40" s="110"/>
-      <c r="AP40" s="110"/>
-      <c r="AQ40" s="110"/>
+      <c r="AK40" s="103"/>
+      <c r="AL40" s="103"/>
+      <c r="AM40" s="103"/>
+      <c r="AN40" s="103"/>
+      <c r="AO40" s="103"/>
+      <c r="AP40" s="103"/>
+      <c r="AQ40" s="103"/>
     </row>
     <row r="41" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
@@ -6817,16 +6817,16 @@
       <c r="AG41" s="17"/>
       <c r="AH41" s="17"/>
       <c r="AI41" s="17"/>
-      <c r="AJ41" s="113" t="s">
+      <c r="AJ41" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="AK41" s="114"/>
-      <c r="AL41" s="114"/>
-      <c r="AM41" s="114"/>
-      <c r="AN41" s="114"/>
-      <c r="AO41" s="114"/>
-      <c r="AP41" s="114"/>
-      <c r="AQ41" s="114"/>
+      <c r="AK41" s="105"/>
+      <c r="AL41" s="105"/>
+      <c r="AM41" s="105"/>
+      <c r="AN41" s="105"/>
+      <c r="AO41" s="105"/>
+      <c r="AP41" s="105"/>
+      <c r="AQ41" s="105"/>
     </row>
     <row r="42" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
@@ -6874,16 +6874,16 @@
       <c r="AG42" s="8"/>
       <c r="AH42" s="8"/>
       <c r="AI42" s="8"/>
-      <c r="AJ42" s="96" t="s">
+      <c r="AJ42" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="AK42" s="110"/>
-      <c r="AL42" s="110"/>
-      <c r="AM42" s="110"/>
-      <c r="AN42" s="110"/>
-      <c r="AO42" s="110"/>
-      <c r="AP42" s="110"/>
-      <c r="AQ42" s="110"/>
+      <c r="AK42" s="103"/>
+      <c r="AL42" s="103"/>
+      <c r="AM42" s="103"/>
+      <c r="AN42" s="103"/>
+      <c r="AO42" s="103"/>
+      <c r="AP42" s="103"/>
+      <c r="AQ42" s="103"/>
     </row>
     <row r="43" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
@@ -6927,16 +6927,16 @@
       <c r="AG43" s="8"/>
       <c r="AH43" s="8"/>
       <c r="AI43" s="8"/>
-      <c r="AJ43" s="96" t="s">
+      <c r="AJ43" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="AK43" s="110"/>
-      <c r="AL43" s="110"/>
-      <c r="AM43" s="110"/>
-      <c r="AN43" s="110"/>
-      <c r="AO43" s="110"/>
-      <c r="AP43" s="110"/>
-      <c r="AQ43" s="110"/>
+      <c r="AK43" s="103"/>
+      <c r="AL43" s="103"/>
+      <c r="AM43" s="103"/>
+      <c r="AN43" s="103"/>
+      <c r="AO43" s="103"/>
+      <c r="AP43" s="103"/>
+      <c r="AQ43" s="103"/>
     </row>
     <row r="44" spans="1:55" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
@@ -6978,16 +6978,16 @@
       <c r="AG44" s="8"/>
       <c r="AH44" s="8"/>
       <c r="AI44" s="8"/>
-      <c r="AJ44" s="96" t="s">
+      <c r="AJ44" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="AK44" s="110"/>
-      <c r="AL44" s="110"/>
-      <c r="AM44" s="110"/>
-      <c r="AN44" s="110"/>
-      <c r="AO44" s="110"/>
-      <c r="AP44" s="110"/>
-      <c r="AQ44" s="110"/>
+      <c r="AK44" s="103"/>
+      <c r="AL44" s="103"/>
+      <c r="AM44" s="103"/>
+      <c r="AN44" s="103"/>
+      <c r="AO44" s="103"/>
+      <c r="AP44" s="103"/>
+      <c r="AQ44" s="103"/>
     </row>
     <row r="45" spans="1:55" x14ac:dyDescent="0.45">
       <c r="BB45" s="70"/>
@@ -6998,43 +6998,43 @@
       <c r="BC46" s="70"/>
     </row>
     <row r="47" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="A47" s="119" t="s">
+      <c r="A47" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="119"/>
-      <c r="C47" s="119"/>
-      <c r="D47" s="119"/>
-      <c r="E47" s="119"/>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
-      <c r="I47" s="119"/>
-      <c r="J47" s="119"/>
-      <c r="K47" s="119"/>
-      <c r="L47" s="119"/>
-      <c r="M47" s="119"/>
-      <c r="N47" s="119"/>
-      <c r="O47" s="119"/>
-      <c r="P47" s="119"/>
-      <c r="Q47" s="119"/>
-      <c r="R47" s="119"/>
-      <c r="S47" s="119"/>
-      <c r="T47" s="119"/>
-      <c r="U47" s="119"/>
-      <c r="V47" s="119"/>
-      <c r="W47" s="119"/>
-      <c r="X47" s="119"/>
-      <c r="Y47" s="119"/>
-      <c r="Z47" s="119"/>
-      <c r="AA47" s="119"/>
-      <c r="AB47" s="119"/>
-      <c r="AC47" s="119"/>
-      <c r="AD47" s="119"/>
-      <c r="AE47" s="119"/>
-      <c r="AF47" s="119"/>
-      <c r="AG47" s="119"/>
-      <c r="AH47" s="119"/>
-      <c r="AI47" s="119"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+      <c r="N47" s="86"/>
+      <c r="O47" s="86"/>
+      <c r="P47" s="86"/>
+      <c r="Q47" s="86"/>
+      <c r="R47" s="86"/>
+      <c r="S47" s="86"/>
+      <c r="T47" s="86"/>
+      <c r="U47" s="86"/>
+      <c r="V47" s="86"/>
+      <c r="W47" s="86"/>
+      <c r="X47" s="86"/>
+      <c r="Y47" s="86"/>
+      <c r="Z47" s="86"/>
+      <c r="AA47" s="86"/>
+      <c r="AB47" s="86"/>
+      <c r="AC47" s="86"/>
+      <c r="AD47" s="86"/>
+      <c r="AE47" s="86"/>
+      <c r="AF47" s="86"/>
+      <c r="AG47" s="86"/>
+      <c r="AH47" s="86"/>
+      <c r="AI47" s="86"/>
       <c r="BB47" s="70"/>
       <c r="BC47" s="70"/>
     </row>
@@ -7149,39 +7149,39 @@
       <c r="B50" s="20">
         <v>1</v>
       </c>
-      <c r="C50" s="106" t="s">
+      <c r="C50" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="107"/>
-      <c r="E50" s="107"/>
-      <c r="F50" s="107"/>
-      <c r="G50" s="107"/>
-      <c r="H50" s="107"/>
-      <c r="I50" s="107"/>
-      <c r="J50" s="107"/>
-      <c r="K50" s="107"/>
-      <c r="L50" s="107"/>
-      <c r="M50" s="107"/>
-      <c r="N50" s="107"/>
-      <c r="O50" s="107"/>
-      <c r="P50" s="107"/>
-      <c r="Q50" s="107"/>
-      <c r="R50" s="107"/>
-      <c r="S50" s="107"/>
-      <c r="T50" s="107"/>
-      <c r="U50" s="107"/>
-      <c r="V50" s="107"/>
-      <c r="W50" s="107"/>
-      <c r="X50" s="107"/>
-      <c r="Y50" s="107"/>
-      <c r="Z50" s="107"/>
-      <c r="AA50" s="107"/>
-      <c r="AB50" s="107"/>
-      <c r="AC50" s="107"/>
-      <c r="AD50" s="107"/>
-      <c r="AE50" s="107"/>
-      <c r="AF50" s="107"/>
-      <c r="AG50" s="108"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="88"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="88"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="88"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="88"/>
+      <c r="O50" s="88"/>
+      <c r="P50" s="88"/>
+      <c r="Q50" s="88"/>
+      <c r="R50" s="88"/>
+      <c r="S50" s="88"/>
+      <c r="T50" s="88"/>
+      <c r="U50" s="88"/>
+      <c r="V50" s="88"/>
+      <c r="W50" s="88"/>
+      <c r="X50" s="88"/>
+      <c r="Y50" s="88"/>
+      <c r="Z50" s="88"/>
+      <c r="AA50" s="88"/>
+      <c r="AB50" s="88"/>
+      <c r="AC50" s="88"/>
+      <c r="AD50" s="88"/>
+      <c r="AE50" s="88"/>
+      <c r="AF50" s="88"/>
+      <c r="AG50" s="89"/>
       <c r="BB50" s="70"/>
       <c r="BC50" s="70"/>
     </row>
@@ -7192,10 +7192,10 @@
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
-      <c r="H51" s="118" t="s">
+      <c r="H51" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="I51" s="118" t="s">
+      <c r="I51" s="83" t="s">
         <v>160</v>
       </c>
       <c r="J51" s="22"/>
@@ -7224,34 +7224,34 @@
       <c r="BC51" s="70"/>
     </row>
     <row r="52" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="91" t="s">
+      <c r="B52" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="91"/>
-      <c r="D52" s="91"/>
-      <c r="E52" s="118" t="s">
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="118"/>
-      <c r="J52" s="91" t="s">
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="83"/>
+      <c r="J52" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="K52" s="91"/>
-      <c r="L52" s="91" t="s">
+      <c r="K52" s="85"/>
+      <c r="L52" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="M52" s="91"/>
-      <c r="N52" s="91" t="s">
+      <c r="M52" s="85"/>
+      <c r="N52" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="O52" s="91"/>
-      <c r="P52" s="91" t="s">
+      <c r="O52" s="85"/>
+      <c r="P52" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="Q52" s="91"/>
+      <c r="Q52" s="85"/>
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
       <c r="T52" s="22"/>
@@ -7272,22 +7272,22 @@
       <c r="BC52" s="70"/>
     </row>
     <row r="53" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="B53" s="91"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="91"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="118"/>
-      <c r="I53" s="118"/>
-      <c r="J53" s="91"/>
-      <c r="K53" s="91"/>
-      <c r="L53" s="91"/>
-      <c r="M53" s="91"/>
-      <c r="N53" s="91"/>
-      <c r="O53" s="91"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="91"/>
+      <c r="B53" s="85"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="83"/>
+      <c r="G53" s="83"/>
+      <c r="H53" s="83"/>
+      <c r="I53" s="83"/>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="85"/>
+      <c r="M53" s="85"/>
+      <c r="N53" s="85"/>
+      <c r="O53" s="85"/>
+      <c r="P53" s="85"/>
+      <c r="Q53" s="85"/>
       <c r="R53" s="22"/>
       <c r="S53" s="22"/>
       <c r="T53" s="22"/>
@@ -7308,22 +7308,22 @@
       <c r="BC53" s="70"/>
     </row>
     <row r="54" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="B54" s="92"/>
-      <c r="C54" s="92"/>
-      <c r="D54" s="92"/>
-      <c r="E54" s="92"/>
-      <c r="F54" s="92"/>
-      <c r="G54" s="92"/>
-      <c r="H54" s="92"/>
-      <c r="I54" s="92"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="92"/>
-      <c r="L54" s="92"/>
-      <c r="M54" s="92"/>
-      <c r="N54" s="92"/>
-      <c r="O54" s="92"/>
-      <c r="P54" s="92"/>
-      <c r="Q54" s="92"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="84"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="84"/>
+      <c r="M54" s="84"/>
+      <c r="N54" s="84"/>
+      <c r="O54" s="84"/>
+      <c r="P54" s="84"/>
+      <c r="Q54" s="84"/>
       <c r="R54" s="22"/>
       <c r="S54" s="22"/>
       <c r="T54" s="22"/>
@@ -7369,29 +7369,29 @@
       <c r="O55" s="24"/>
       <c r="P55" s="20"/>
       <c r="Q55" s="24"/>
-      <c r="R55" s="106" t="s">
+      <c r="R55" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="S55" s="107"/>
-      <c r="T55" s="107"/>
-      <c r="U55" s="107"/>
-      <c r="V55" s="107"/>
-      <c r="W55" s="107"/>
-      <c r="X55" s="107"/>
-      <c r="Y55" s="107"/>
-      <c r="Z55" s="107"/>
-      <c r="AA55" s="107"/>
-      <c r="AB55" s="107"/>
-      <c r="AC55" s="107"/>
-      <c r="AD55" s="107"/>
-      <c r="AE55" s="107"/>
-      <c r="AF55" s="107"/>
-      <c r="AG55" s="108"/>
-      <c r="AJ55" s="110"/>
-      <c r="AK55" s="110"/>
-      <c r="AL55" s="110"/>
-      <c r="AM55" s="110"/>
-      <c r="AN55" s="110"/>
+      <c r="S55" s="88"/>
+      <c r="T55" s="88"/>
+      <c r="U55" s="88"/>
+      <c r="V55" s="88"/>
+      <c r="W55" s="88"/>
+      <c r="X55" s="88"/>
+      <c r="Y55" s="88"/>
+      <c r="Z55" s="88"/>
+      <c r="AA55" s="88"/>
+      <c r="AB55" s="88"/>
+      <c r="AC55" s="88"/>
+      <c r="AD55" s="88"/>
+      <c r="AE55" s="88"/>
+      <c r="AF55" s="88"/>
+      <c r="AG55" s="89"/>
+      <c r="AJ55" s="103"/>
+      <c r="AK55" s="103"/>
+      <c r="AL55" s="103"/>
+      <c r="AM55" s="103"/>
+      <c r="AN55" s="103"/>
       <c r="AR55" s="51"/>
       <c r="AS55" s="51"/>
       <c r="BB55" s="70"/>
@@ -7401,10 +7401,10 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="H56" s="118" t="s">
+      <c r="H56" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="I56" s="118" t="s">
+      <c r="I56" s="83" t="s">
         <v>160</v>
       </c>
       <c r="J56" s="28"/>
@@ -7432,136 +7432,136 @@
       <c r="BC56" s="70"/>
     </row>
     <row r="57" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="91" t="s">
+      <c r="B57" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91"/>
-      <c r="E57" s="118" t="s">
+      <c r="C57" s="85"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="F57" s="118"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="118"/>
-      <c r="I57" s="118"/>
-      <c r="J57" s="91" t="s">
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="83"/>
+      <c r="J57" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="91"/>
-      <c r="L57" s="91" t="s">
+      <c r="K57" s="85"/>
+      <c r="L57" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="M57" s="91"/>
-      <c r="N57" s="91" t="s">
+      <c r="M57" s="85"/>
+      <c r="N57" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="O57" s="91"/>
-      <c r="P57" s="91" t="s">
+      <c r="O57" s="85"/>
+      <c r="P57" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="Q57" s="91"/>
-      <c r="R57" s="91" t="s">
+      <c r="Q57" s="85"/>
+      <c r="R57" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S57" s="91"/>
-      <c r="T57" s="91"/>
-      <c r="U57" s="91"/>
-      <c r="V57" s="91"/>
-      <c r="W57" s="91" t="s">
+      <c r="S57" s="85"/>
+      <c r="T57" s="85"/>
+      <c r="U57" s="85"/>
+      <c r="V57" s="85"/>
+      <c r="W57" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="X57" s="91"/>
-      <c r="Y57" s="91" t="s">
+      <c r="X57" s="85"/>
+      <c r="Y57" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="Z57" s="91"/>
-      <c r="AA57" s="91" t="s">
+      <c r="Z57" s="85"/>
+      <c r="AA57" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="AB57" s="91"/>
-      <c r="AC57" s="91" t="s">
+      <c r="AB57" s="85"/>
+      <c r="AC57" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="AD57" s="91"/>
-      <c r="AE57" s="91"/>
-      <c r="AF57" s="91"/>
-      <c r="AG57" s="91"/>
+      <c r="AD57" s="85"/>
+      <c r="AE57" s="85"/>
+      <c r="AF57" s="85"/>
+      <c r="AG57" s="85"/>
       <c r="AR57" s="51"/>
       <c r="AS57" s="51"/>
       <c r="BB57" s="70"/>
       <c r="BC57" s="70"/>
     </row>
     <row r="58" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="B58" s="91"/>
-      <c r="C58" s="91"/>
-      <c r="D58" s="91"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="118"/>
-      <c r="G58" s="118"/>
-      <c r="H58" s="118"/>
-      <c r="I58" s="118"/>
-      <c r="J58" s="91"/>
-      <c r="K58" s="91"/>
-      <c r="L58" s="91"/>
-      <c r="M58" s="91"/>
-      <c r="N58" s="91"/>
-      <c r="O58" s="91"/>
-      <c r="P58" s="91"/>
-      <c r="Q58" s="91"/>
-      <c r="R58" s="91"/>
-      <c r="S58" s="91"/>
-      <c r="T58" s="91"/>
-      <c r="U58" s="91"/>
-      <c r="V58" s="91"/>
-      <c r="W58" s="91"/>
-      <c r="X58" s="91"/>
-      <c r="Y58" s="91"/>
-      <c r="Z58" s="91"/>
-      <c r="AA58" s="91"/>
-      <c r="AB58" s="91"/>
-      <c r="AC58" s="91"/>
-      <c r="AD58" s="91"/>
-      <c r="AE58" s="91"/>
-      <c r="AF58" s="91"/>
-      <c r="AG58" s="91"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="83"/>
+      <c r="H58" s="83"/>
+      <c r="I58" s="83"/>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="85"/>
+      <c r="N58" s="85"/>
+      <c r="O58" s="85"/>
+      <c r="P58" s="85"/>
+      <c r="Q58" s="85"/>
+      <c r="R58" s="85"/>
+      <c r="S58" s="85"/>
+      <c r="T58" s="85"/>
+      <c r="U58" s="85"/>
+      <c r="V58" s="85"/>
+      <c r="W58" s="85"/>
+      <c r="X58" s="85"/>
+      <c r="Y58" s="85"/>
+      <c r="Z58" s="85"/>
+      <c r="AA58" s="85"/>
+      <c r="AB58" s="85"/>
+      <c r="AC58" s="85"/>
+      <c r="AD58" s="85"/>
+      <c r="AE58" s="85"/>
+      <c r="AF58" s="85"/>
+      <c r="AG58" s="85"/>
       <c r="AR58" s="51"/>
       <c r="AS58" s="51"/>
       <c r="BB58" s="70"/>
       <c r="BC58" s="70"/>
     </row>
     <row r="59" spans="1:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B59" s="92"/>
-      <c r="C59" s="92"/>
-      <c r="D59" s="92"/>
-      <c r="E59" s="92"/>
-      <c r="F59" s="92"/>
-      <c r="G59" s="92"/>
-      <c r="H59" s="92"/>
-      <c r="I59" s="92"/>
-      <c r="J59" s="92"/>
-      <c r="K59" s="92"/>
-      <c r="L59" s="92"/>
-      <c r="M59" s="92"/>
-      <c r="N59" s="92"/>
-      <c r="O59" s="92"/>
-      <c r="P59" s="92"/>
-      <c r="Q59" s="92"/>
-      <c r="R59" s="92"/>
-      <c r="S59" s="92"/>
-      <c r="T59" s="92"/>
-      <c r="U59" s="92"/>
-      <c r="V59" s="92"/>
-      <c r="W59" s="92"/>
-      <c r="X59" s="92"/>
-      <c r="Y59" s="92"/>
-      <c r="Z59" s="92"/>
-      <c r="AA59" s="92"/>
-      <c r="AB59" s="92"/>
-      <c r="AC59" s="92"/>
-      <c r="AD59" s="92"/>
-      <c r="AE59" s="92"/>
-      <c r="AF59" s="92"/>
-      <c r="AG59" s="92"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="84"/>
+      <c r="J59" s="84"/>
+      <c r="K59" s="84"/>
+      <c r="L59" s="84"/>
+      <c r="M59" s="84"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
+      <c r="P59" s="84"/>
+      <c r="Q59" s="84"/>
+      <c r="R59" s="84"/>
+      <c r="S59" s="84"/>
+      <c r="T59" s="84"/>
+      <c r="U59" s="84"/>
+      <c r="V59" s="84"/>
+      <c r="W59" s="84"/>
+      <c r="X59" s="84"/>
+      <c r="Y59" s="84"/>
+      <c r="Z59" s="84"/>
+      <c r="AA59" s="84"/>
+      <c r="AB59" s="84"/>
+      <c r="AC59" s="84"/>
+      <c r="AD59" s="84"/>
+      <c r="AE59" s="84"/>
+      <c r="AF59" s="84"/>
+      <c r="AG59" s="84"/>
       <c r="BB59" s="70"/>
       <c r="BC59" s="70"/>
     </row>
@@ -7607,11 +7607,11 @@
       <c r="AE60" s="26"/>
       <c r="AF60" s="26"/>
       <c r="AG60" s="27"/>
-      <c r="AN60" s="77" t="s">
+      <c r="AN60" s="112" t="s">
         <v>115</v>
       </c>
       <c r="AX60" s="34"/>
-      <c r="AY60" s="77" t="s">
+      <c r="AY60" s="112" t="s">
         <v>115</v>
       </c>
       <c r="AZ60" s="34"/>
@@ -7624,19 +7624,19 @@
       <c r="AM61" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="AN61" s="78"/>
+      <c r="AN61" s="113"/>
       <c r="AO61" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="AQ61" s="85" t="s">
+      <c r="AQ61" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="AR61" s="86"/>
+      <c r="AR61" s="118"/>
       <c r="AU61" s="34"/>
       <c r="AX61" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="AY61" s="78"/>
+      <c r="AY61" s="113"/>
       <c r="AZ61" s="52" t="s">
         <v>117</v>
       </c>
@@ -7644,43 +7644,43 @@
       <c r="BC61" s="70"/>
     </row>
     <row r="62" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="B62" s="98" t="s">
+      <c r="B62" s="92" t="s">
         <v>161</v>
       </c>
-      <c r="C62" s="121"/>
-      <c r="D62" s="99"/>
-      <c r="E62" s="95" t="s">
+      <c r="C62" s="93"/>
+      <c r="D62" s="94"/>
+      <c r="E62" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F62" s="95" t="s">
+      <c r="F62" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="G62" s="95" t="s">
+      <c r="G62" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="H62" s="95" t="s">
+      <c r="H62" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="I62" s="95" t="s">
+      <c r="I62" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="J62" s="109" t="s">
+      <c r="J62" s="111" t="s">
         <v>166</v>
       </c>
-      <c r="K62" s="95" t="s">
+      <c r="K62" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="M62" s="98" t="s">
+      <c r="M62" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="N62" s="99"/>
-      <c r="O62" s="95" t="s">
+      <c r="N62" s="94"/>
+      <c r="O62" s="91" t="s">
         <v>162</v>
       </c>
-      <c r="P62" s="95" t="s">
+      <c r="P62" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="Q62" s="105" t="s">
+      <c r="Q62" s="90" t="s">
         <v>105</v>
       </c>
       <c r="T62" s="21">
@@ -7701,40 +7701,40 @@
       <c r="Y62" s="19">
         <v>0</v>
       </c>
-      <c r="Z62" s="94" t="s">
+      <c r="Z62" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="AA62" s="94"/>
-      <c r="AB62" s="94"/>
+      <c r="AA62" s="79"/>
+      <c r="AB62" s="79"/>
       <c r="AC62" s="6"/>
       <c r="AD62" s="6"/>
       <c r="AE62" s="6"/>
       <c r="AF62" s="6"/>
-      <c r="AN62" s="78"/>
-      <c r="AQ62" s="87"/>
-      <c r="AR62" s="88"/>
+      <c r="AN62" s="113"/>
+      <c r="AQ62" s="119"/>
+      <c r="AR62" s="120"/>
       <c r="AX62" s="34"/>
-      <c r="AY62" s="78"/>
+      <c r="AY62" s="113"/>
       <c r="AZ62" s="34"/>
       <c r="BB62" s="70"/>
       <c r="BC62" s="70"/>
     </row>
     <row r="63" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="100"/>
-      <c r="C63" s="122"/>
-      <c r="D63" s="101"/>
-      <c r="E63" s="95"/>
-      <c r="F63" s="95"/>
-      <c r="G63" s="95"/>
-      <c r="H63" s="95"/>
-      <c r="I63" s="95"/>
-      <c r="J63" s="109"/>
-      <c r="K63" s="95"/>
-      <c r="M63" s="100"/>
-      <c r="N63" s="101"/>
-      <c r="O63" s="95"/>
-      <c r="P63" s="95"/>
-      <c r="Q63" s="105"/>
+      <c r="B63" s="95"/>
+      <c r="C63" s="96"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="91"/>
+      <c r="F63" s="91"/>
+      <c r="G63" s="91"/>
+      <c r="H63" s="91"/>
+      <c r="I63" s="91"/>
+      <c r="J63" s="111"/>
+      <c r="K63" s="91"/>
+      <c r="M63" s="95"/>
+      <c r="N63" s="97"/>
+      <c r="O63" s="91"/>
+      <c r="P63" s="91"/>
+      <c r="Q63" s="90"/>
       <c r="T63" s="21">
         <v>0</v>
       </c>
@@ -7753,11 +7753,11 @@
       <c r="Y63" s="19">
         <v>1</v>
       </c>
-      <c r="Z63" s="94" t="s">
+      <c r="Z63" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="AA63" s="94"/>
-      <c r="AB63" s="94"/>
+      <c r="AA63" s="79"/>
+      <c r="AB63" s="79"/>
       <c r="AC63" s="6"/>
       <c r="AD63" s="6"/>
       <c r="AE63" s="6"/>
@@ -7765,31 +7765,31 @@
       <c r="AG63" s="6"/>
       <c r="AH63" s="6"/>
       <c r="AI63" s="6"/>
-      <c r="AN63" s="78"/>
-      <c r="AQ63" s="87"/>
-      <c r="AR63" s="88"/>
+      <c r="AN63" s="113"/>
+      <c r="AQ63" s="119"/>
+      <c r="AR63" s="120"/>
       <c r="AX63" s="34"/>
-      <c r="AY63" s="78"/>
+      <c r="AY63" s="113"/>
       <c r="AZ63" s="34"/>
       <c r="BB63" s="70"/>
       <c r="BC63" s="70"/>
     </row>
     <row r="64" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B64" s="100"/>
-      <c r="C64" s="122"/>
-      <c r="D64" s="101"/>
-      <c r="E64" s="95"/>
-      <c r="F64" s="95"/>
-      <c r="G64" s="95"/>
-      <c r="H64" s="95"/>
-      <c r="I64" s="95"/>
-      <c r="J64" s="109"/>
-      <c r="K64" s="95"/>
-      <c r="M64" s="100"/>
-      <c r="N64" s="101"/>
-      <c r="O64" s="95"/>
-      <c r="P64" s="95"/>
-      <c r="Q64" s="105"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="96"/>
+      <c r="D64" s="97"/>
+      <c r="E64" s="91"/>
+      <c r="F64" s="91"/>
+      <c r="G64" s="91"/>
+      <c r="H64" s="91"/>
+      <c r="I64" s="91"/>
+      <c r="J64" s="111"/>
+      <c r="K64" s="91"/>
+      <c r="M64" s="95"/>
+      <c r="N64" s="97"/>
+      <c r="O64" s="91"/>
+      <c r="P64" s="91"/>
+      <c r="Q64" s="90"/>
       <c r="T64" s="21">
         <v>0</v>
       </c>
@@ -7808,11 +7808,11 @@
       <c r="Y64" s="19">
         <v>2</v>
       </c>
-      <c r="Z64" s="76" t="s">
+      <c r="Z64" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="AA64" s="76"/>
-      <c r="AB64" s="76"/>
+      <c r="AA64" s="78"/>
+      <c r="AB64" s="78"/>
       <c r="AC64" s="6"/>
       <c r="AD64" s="6"/>
       <c r="AE64" s="6"/>
@@ -7820,31 +7820,31 @@
       <c r="AG64" s="6"/>
       <c r="AH64" s="6"/>
       <c r="AI64" s="6"/>
-      <c r="AN64" s="78"/>
-      <c r="AQ64" s="89"/>
-      <c r="AR64" s="90"/>
+      <c r="AN64" s="113"/>
+      <c r="AQ64" s="121"/>
+      <c r="AR64" s="122"/>
       <c r="AX64" s="34"/>
-      <c r="AY64" s="78"/>
+      <c r="AY64" s="113"/>
       <c r="AZ64" s="34"/>
       <c r="BB64" s="70"/>
       <c r="BC64" s="70"/>
     </row>
     <row r="65" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="102"/>
-      <c r="C65" s="123"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="95"/>
-      <c r="F65" s="95"/>
-      <c r="G65" s="95"/>
-      <c r="H65" s="95"/>
-      <c r="I65" s="95"/>
-      <c r="J65" s="109"/>
-      <c r="K65" s="95"/>
-      <c r="M65" s="102"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="95"/>
-      <c r="P65" s="95"/>
-      <c r="Q65" s="105"/>
+      <c r="B65" s="98"/>
+      <c r="C65" s="99"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="91"/>
+      <c r="F65" s="91"/>
+      <c r="G65" s="91"/>
+      <c r="H65" s="91"/>
+      <c r="I65" s="91"/>
+      <c r="J65" s="111"/>
+      <c r="K65" s="91"/>
+      <c r="M65" s="98"/>
+      <c r="N65" s="100"/>
+      <c r="O65" s="91"/>
+      <c r="P65" s="91"/>
+      <c r="Q65" s="90"/>
       <c r="T65" s="21">
         <v>0</v>
       </c>
@@ -7863,11 +7863,11 @@
       <c r="Y65" s="19">
         <v>3</v>
       </c>
-      <c r="Z65" s="76" t="s">
+      <c r="Z65" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="AA65" s="76"/>
-      <c r="AB65" s="76"/>
+      <c r="AA65" s="78"/>
+      <c r="AB65" s="78"/>
       <c r="AC65" s="6"/>
       <c r="AD65" s="6"/>
       <c r="AE65" s="6"/>
@@ -7875,9 +7875,9 @@
       <c r="AG65" s="6"/>
       <c r="AH65" s="6"/>
       <c r="AI65" s="6"/>
-      <c r="AN65" s="78"/>
+      <c r="AN65" s="113"/>
       <c r="AX65" s="34"/>
-      <c r="AY65" s="78"/>
+      <c r="AY65" s="113"/>
       <c r="AZ65" s="34"/>
       <c r="BB65" s="70"/>
       <c r="BC65" s="70"/>
@@ -7926,11 +7926,11 @@
       <c r="Y66" s="19">
         <v>4</v>
       </c>
-      <c r="Z66" s="76" t="s">
+      <c r="Z66" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="AA66" s="76"/>
-      <c r="AB66" s="76"/>
+      <c r="AA66" s="78"/>
+      <c r="AB66" s="78"/>
       <c r="AC66" s="6"/>
       <c r="AD66" s="6"/>
       <c r="AE66" s="6"/>
@@ -7938,11 +7938,11 @@
       <c r="AG66" s="6"/>
       <c r="AH66" s="6"/>
       <c r="AI66" s="6"/>
-      <c r="AN66" s="78"/>
+      <c r="AN66" s="113"/>
       <c r="AR66" s="15"/>
       <c r="AS66" s="15"/>
       <c r="AX66" s="34"/>
-      <c r="AY66" s="78"/>
+      <c r="AY66" s="113"/>
       <c r="AZ66" s="34"/>
       <c r="BB66" s="70"/>
       <c r="BC66" s="70"/>
@@ -7995,11 +7995,11 @@
       <c r="Y67" s="19">
         <v>5</v>
       </c>
-      <c r="Z67" s="76" t="s">
+      <c r="Z67" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="AA67" s="76"/>
-      <c r="AB67" s="76"/>
+      <c r="AA67" s="78"/>
+      <c r="AB67" s="78"/>
       <c r="AC67" s="6"/>
       <c r="AD67" s="6"/>
       <c r="AE67" s="6"/>
@@ -8007,9 +8007,9 @@
       <c r="AG67" s="6"/>
       <c r="AH67" s="6"/>
       <c r="AI67" s="6"/>
-      <c r="AN67" s="78"/>
+      <c r="AN67" s="113"/>
       <c r="AX67" s="34"/>
-      <c r="AY67" s="78"/>
+      <c r="AY67" s="113"/>
       <c r="AZ67" s="34"/>
       <c r="BB67" s="70"/>
       <c r="BC67" s="70"/>
@@ -8067,11 +8067,11 @@
       <c r="Y68" s="19">
         <v>6</v>
       </c>
-      <c r="Z68" s="76" t="s">
+      <c r="Z68" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="AA68" s="76"/>
-      <c r="AB68" s="76"/>
+      <c r="AA68" s="78"/>
+      <c r="AB68" s="78"/>
       <c r="AC68" s="6"/>
       <c r="AD68" s="6"/>
       <c r="AE68" s="6"/>
@@ -8079,9 +8079,9 @@
       <c r="AG68" s="6"/>
       <c r="AH68" s="6"/>
       <c r="AI68" s="6"/>
-      <c r="AN68" s="78"/>
+      <c r="AN68" s="113"/>
       <c r="AX68" s="34"/>
-      <c r="AY68" s="78"/>
+      <c r="AY68" s="113"/>
       <c r="AZ68" s="34"/>
       <c r="BB68" s="70"/>
       <c r="BC68" s="70"/>
@@ -8138,11 +8138,11 @@
       <c r="Y69" s="19">
         <v>7</v>
       </c>
-      <c r="Z69" s="76" t="s">
+      <c r="Z69" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="AA69" s="76"/>
-      <c r="AB69" s="76"/>
+      <c r="AA69" s="78"/>
+      <c r="AB69" s="78"/>
       <c r="AC69" s="6"/>
       <c r="AD69" s="6"/>
       <c r="AE69" s="6"/>
@@ -8150,11 +8150,11 @@
       <c r="AG69" s="6"/>
       <c r="AH69" s="6"/>
       <c r="AI69" s="6"/>
-      <c r="AN69" s="78"/>
+      <c r="AN69" s="113"/>
       <c r="AX69" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="AY69" s="78"/>
+      <c r="AY69" s="113"/>
       <c r="AZ69" s="34"/>
       <c r="BB69" s="70"/>
       <c r="BC69" s="70"/>
@@ -8198,11 +8198,11 @@
       <c r="Y70" s="19">
         <v>8</v>
       </c>
-      <c r="Z70" s="76" t="s">
+      <c r="Z70" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="AA70" s="76"/>
-      <c r="AB70" s="76"/>
+      <c r="AA70" s="78"/>
+      <c r="AB70" s="78"/>
       <c r="AC70" s="6"/>
       <c r="AD70" s="6"/>
       <c r="AE70" s="6"/>
@@ -8210,9 +8210,9 @@
       <c r="AG70" s="6"/>
       <c r="AH70" s="6"/>
       <c r="AI70" s="6"/>
-      <c r="AN70" s="78"/>
+      <c r="AN70" s="113"/>
       <c r="AX70" s="34"/>
-      <c r="AY70" s="78"/>
+      <c r="AY70" s="113"/>
       <c r="AZ70" s="34"/>
       <c r="BB70" s="70"/>
       <c r="BC70" s="70"/>
@@ -8237,17 +8237,17 @@
       <c r="K71" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="M71" s="98" t="s">
+      <c r="M71" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="N71" s="99"/>
-      <c r="O71" s="93" t="s">
+      <c r="N71" s="94"/>
+      <c r="O71" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="P71" s="93" t="s">
+      <c r="P71" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="Q71" s="93" t="s">
+      <c r="Q71" s="101" t="s">
         <v>165</v>
       </c>
       <c r="R71" s="6"/>
@@ -8269,11 +8269,11 @@
       <c r="Y71" s="19">
         <v>9</v>
       </c>
-      <c r="Z71" s="76" t="s">
+      <c r="Z71" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="AA71" s="76"/>
-      <c r="AB71" s="76"/>
+      <c r="AA71" s="78"/>
+      <c r="AB71" s="78"/>
       <c r="AC71" s="6"/>
       <c r="AD71" s="6"/>
       <c r="AE71" s="6"/>
@@ -8284,22 +8284,22 @@
       <c r="AM71" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="AN71" s="78"/>
+      <c r="AN71" s="113"/>
       <c r="AO71" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="AQ71" s="80" t="s">
+      <c r="AQ71" s="123" t="s">
         <v>139</v>
       </c>
-      <c r="AR71" s="81"/>
-      <c r="AU71" s="80" t="s">
+      <c r="AR71" s="124"/>
+      <c r="AU71" s="123" t="s">
         <v>140</v>
       </c>
-      <c r="AV71" s="81"/>
+      <c r="AV71" s="124"/>
       <c r="AX71" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="AY71" s="78"/>
+      <c r="AY71" s="113"/>
       <c r="AZ71" s="52" t="s">
         <v>120</v>
       </c>
@@ -8325,11 +8325,11 @@
       </c>
       <c r="J72" s="61"/>
       <c r="K72" s="62"/>
-      <c r="M72" s="100"/>
-      <c r="N72" s="101"/>
-      <c r="O72" s="93"/>
-      <c r="P72" s="93"/>
-      <c r="Q72" s="93"/>
+      <c r="M72" s="95"/>
+      <c r="N72" s="97"/>
+      <c r="O72" s="101"/>
+      <c r="P72" s="101"/>
+      <c r="Q72" s="101"/>
       <c r="R72" s="6"/>
       <c r="T72" s="21">
         <v>0</v>
@@ -8349,11 +8349,11 @@
       <c r="Y72" s="19">
         <v>10</v>
       </c>
-      <c r="Z72" s="76" t="s">
+      <c r="Z72" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="AA72" s="76"/>
-      <c r="AB72" s="76"/>
+      <c r="AA72" s="78"/>
+      <c r="AB72" s="78"/>
       <c r="AC72" s="6"/>
       <c r="AD72" s="6"/>
       <c r="AE72" s="6"/>
@@ -8361,9 +8361,9 @@
       <c r="AG72" s="6"/>
       <c r="AH72" s="6"/>
       <c r="AI72" s="6"/>
-      <c r="AN72" s="79"/>
+      <c r="AN72" s="114"/>
       <c r="AX72" s="34"/>
-      <c r="AY72" s="79"/>
+      <c r="AY72" s="114"/>
       <c r="AZ72" s="34"/>
       <c r="BB72" s="70"/>
       <c r="BC72" s="70"/>
@@ -8387,11 +8387,11 @@
         <v>59</v>
       </c>
       <c r="K73" s="62"/>
-      <c r="M73" s="100"/>
-      <c r="N73" s="101"/>
-      <c r="O73" s="93"/>
-      <c r="P73" s="93"/>
-      <c r="Q73" s="93"/>
+      <c r="M73" s="95"/>
+      <c r="N73" s="97"/>
+      <c r="O73" s="101"/>
+      <c r="P73" s="101"/>
+      <c r="Q73" s="101"/>
       <c r="R73" s="6"/>
       <c r="T73" s="21">
         <v>0</v>
@@ -8411,11 +8411,11 @@
       <c r="Y73" s="19">
         <v>11</v>
       </c>
-      <c r="Z73" s="76" t="s">
+      <c r="Z73" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="AA73" s="76"/>
-      <c r="AB73" s="76"/>
+      <c r="AA73" s="78"/>
+      <c r="AB73" s="78"/>
       <c r="AC73" s="6"/>
       <c r="AD73" s="6"/>
       <c r="AE73" s="6"/>
@@ -8434,11 +8434,11 @@
       <c r="E74" s="6"/>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
-      <c r="M74" s="100"/>
-      <c r="N74" s="101"/>
-      <c r="O74" s="93"/>
-      <c r="P74" s="93"/>
-      <c r="Q74" s="93"/>
+      <c r="M74" s="95"/>
+      <c r="N74" s="97"/>
+      <c r="O74" s="101"/>
+      <c r="P74" s="101"/>
+      <c r="Q74" s="101"/>
       <c r="R74" s="6"/>
       <c r="T74" s="21">
         <v>0</v>
@@ -8458,11 +8458,11 @@
       <c r="Y74" s="19">
         <v>12</v>
       </c>
-      <c r="Z74" s="76" t="s">
+      <c r="Z74" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="AA74" s="76"/>
-      <c r="AB74" s="76"/>
+      <c r="AA74" s="78"/>
+      <c r="AB74" s="78"/>
       <c r="AC74" s="6"/>
       <c r="AD74" s="6"/>
       <c r="AE74" s="6"/>
@@ -8489,11 +8489,11 @@
       <c r="F75" s="6"/>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
-      <c r="M75" s="100"/>
-      <c r="N75" s="101"/>
-      <c r="O75" s="93"/>
-      <c r="P75" s="93"/>
-      <c r="Q75" s="93"/>
+      <c r="M75" s="95"/>
+      <c r="N75" s="97"/>
+      <c r="O75" s="101"/>
+      <c r="P75" s="101"/>
+      <c r="Q75" s="101"/>
       <c r="R75" s="6"/>
       <c r="T75" s="21">
         <v>0</v>
@@ -8513,11 +8513,11 @@
       <c r="Y75" s="19">
         <v>13</v>
       </c>
-      <c r="Z75" s="76" t="s">
+      <c r="Z75" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="AA75" s="76"/>
-      <c r="AB75" s="76"/>
+      <c r="AA75" s="78"/>
+      <c r="AB75" s="78"/>
       <c r="AC75" s="6"/>
       <c r="AD75" s="6"/>
       <c r="AE75" s="6"/>
@@ -8544,11 +8544,11 @@
       <c r="F76" s="6"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
-      <c r="M76" s="102"/>
-      <c r="N76" s="103"/>
-      <c r="O76" s="93"/>
-      <c r="P76" s="93"/>
-      <c r="Q76" s="93"/>
+      <c r="M76" s="98"/>
+      <c r="N76" s="100"/>
+      <c r="O76" s="101"/>
+      <c r="P76" s="101"/>
+      <c r="Q76" s="101"/>
       <c r="R76" s="6"/>
       <c r="T76" s="21">
         <v>0</v>
@@ -8568,11 +8568,11 @@
       <c r="Y76" s="19">
         <v>14</v>
       </c>
-      <c r="Z76" s="76" t="s">
+      <c r="Z76" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="AA76" s="76"/>
-      <c r="AB76" s="76"/>
+      <c r="AA76" s="78"/>
+      <c r="AB76" s="78"/>
       <c r="AC76" s="6"/>
       <c r="AD76" s="6"/>
       <c r="AE76" s="6"/>
@@ -8595,17 +8595,17 @@
       <c r="BC76" s="70"/>
     </row>
     <row r="77" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B77" s="98" t="s">
+      <c r="B77" s="92" t="s">
         <v>136</v>
       </c>
-      <c r="C77" s="99"/>
-      <c r="D77" s="95" t="s">
+      <c r="C77" s="94"/>
+      <c r="D77" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="E77" s="95" t="s">
+      <c r="E77" s="91" t="s">
         <v>164</v>
       </c>
-      <c r="F77" s="105" t="s">
+      <c r="F77" s="90" t="s">
         <v>141</v>
       </c>
       <c r="H77" s="6"/>
@@ -8638,11 +8638,11 @@
       <c r="Y77" s="19">
         <v>15</v>
       </c>
-      <c r="Z77" s="76" t="s">
+      <c r="Z77" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="AA77" s="76"/>
-      <c r="AB77" s="76"/>
+      <c r="AA77" s="78"/>
+      <c r="AB77" s="78"/>
       <c r="AC77" s="6"/>
       <c r="AD77" s="6"/>
       <c r="AE77" s="6"/>
@@ -8656,11 +8656,11 @@
       <c r="BC77" s="70"/>
     </row>
     <row r="78" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B78" s="100"/>
-      <c r="C78" s="101"/>
-      <c r="D78" s="95"/>
-      <c r="E78" s="95"/>
-      <c r="F78" s="105"/>
+      <c r="B78" s="95"/>
+      <c r="C78" s="97"/>
+      <c r="D78" s="91"/>
+      <c r="E78" s="91"/>
+      <c r="F78" s="90"/>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
       <c r="M78" s="20">
@@ -8693,41 +8693,41 @@
       <c r="Y78" s="19">
         <v>16</v>
       </c>
-      <c r="Z78" s="76" t="s">
+      <c r="Z78" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="AA78" s="76"/>
-      <c r="AB78" s="76"/>
+      <c r="AA78" s="78"/>
+      <c r="AB78" s="78"/>
       <c r="AC78" s="6"/>
       <c r="AD78" s="6"/>
       <c r="AE78" s="6"/>
       <c r="AF78" s="6"/>
       <c r="AI78" s="6"/>
-      <c r="AN78" s="82" t="s">
+      <c r="AN78" s="115" t="s">
         <v>125</v>
       </c>
-      <c r="AO78" s="83"/>
-      <c r="AQ78" s="85" t="s">
+      <c r="AO78" s="116"/>
+      <c r="AQ78" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="AR78" s="86"/>
+      <c r="AR78" s="118"/>
       <c r="AT78" s="34"/>
       <c r="AV78" s="15"/>
       <c r="AW78" s="15"/>
-      <c r="AX78" s="82" t="s">
+      <c r="AX78" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="AY78" s="83"/>
+      <c r="AY78" s="116"/>
       <c r="AZ78" s="34"/>
       <c r="BB78" s="70"/>
       <c r="BC78" s="70"/>
     </row>
     <row r="79" spans="1:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B79" s="102"/>
-      <c r="C79" s="103"/>
-      <c r="D79" s="95"/>
-      <c r="E79" s="95"/>
-      <c r="F79" s="105"/>
+      <c r="B79" s="98"/>
+      <c r="C79" s="100"/>
+      <c r="D79" s="91"/>
+      <c r="E79" s="91"/>
+      <c r="F79" s="90"/>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
       <c r="M79" s="20">
@@ -8760,11 +8760,11 @@
       <c r="Y79" s="19">
         <v>17</v>
       </c>
-      <c r="Z79" s="76" t="s">
+      <c r="Z79" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="AA79" s="76"/>
-      <c r="AB79" s="76"/>
+      <c r="AA79" s="78"/>
+      <c r="AB79" s="78"/>
       <c r="AC79" s="6"/>
       <c r="AD79" s="6"/>
       <c r="AE79" s="6"/>
@@ -8776,8 +8776,8 @@
       <c r="AO79" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="AQ79" s="87"/>
-      <c r="AR79" s="88"/>
+      <c r="AQ79" s="119"/>
+      <c r="AR79" s="120"/>
       <c r="AV79" s="15"/>
       <c r="AW79" s="15"/>
       <c r="AX79" s="53" t="s">
@@ -8832,18 +8832,18 @@
       <c r="Y80" s="19">
         <v>18</v>
       </c>
-      <c r="Z80" s="76" t="s">
+      <c r="Z80" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="AA80" s="76"/>
-      <c r="AB80" s="76"/>
+      <c r="AA80" s="78"/>
+      <c r="AB80" s="78"/>
       <c r="AC80" s="6"/>
       <c r="AD80" s="6"/>
       <c r="AE80" s="6"/>
       <c r="AF80" s="6"/>
       <c r="AI80" s="6"/>
-      <c r="AQ80" s="87"/>
-      <c r="AR80" s="88"/>
+      <c r="AQ80" s="119"/>
+      <c r="AR80" s="120"/>
       <c r="AV80" s="34"/>
       <c r="AX80" s="34"/>
       <c r="AY80" s="34"/>
@@ -8881,24 +8881,24 @@
       <c r="Y81" s="19">
         <v>19</v>
       </c>
-      <c r="Z81" s="76" t="s">
+      <c r="Z81" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="AA81" s="76"/>
-      <c r="AB81" s="76"/>
+      <c r="AA81" s="78"/>
+      <c r="AB81" s="78"/>
       <c r="AC81" s="6"/>
       <c r="AD81" s="6"/>
       <c r="AE81" s="6"/>
       <c r="AF81" s="6"/>
       <c r="AI81" s="6"/>
-      <c r="AN81" s="77" t="s">
+      <c r="AN81" s="112" t="s">
         <v>123</v>
       </c>
-      <c r="AQ81" s="89"/>
-      <c r="AR81" s="90"/>
+      <c r="AQ81" s="121"/>
+      <c r="AR81" s="122"/>
       <c r="AV81" s="34"/>
       <c r="AX81" s="34"/>
-      <c r="AY81" s="77" t="s">
+      <c r="AY81" s="112" t="s">
         <v>129</v>
       </c>
       <c r="AZ81" s="34"/>
@@ -8919,17 +8919,17 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
-      <c r="M82" s="98" t="s">
+      <c r="M82" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="N82" s="99"/>
-      <c r="O82" s="95" t="s">
+      <c r="N82" s="94"/>
+      <c r="O82" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="P82" s="95" t="s">
+      <c r="P82" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="Q82" s="104" t="s">
+      <c r="Q82" s="110" t="s">
         <v>101</v>
       </c>
       <c r="T82" s="21">
@@ -8950,18 +8950,18 @@
       <c r="Y82" s="19">
         <v>20</v>
       </c>
-      <c r="Z82" s="94"/>
-      <c r="AA82" s="94"/>
-      <c r="AB82" s="94"/>
+      <c r="Z82" s="79"/>
+      <c r="AA82" s="79"/>
+      <c r="AB82" s="79"/>
       <c r="AC82" s="6"/>
       <c r="AD82" s="6"/>
       <c r="AE82" s="6"/>
       <c r="AF82" s="6"/>
       <c r="AI82" s="6"/>
-      <c r="AN82" s="78"/>
+      <c r="AN82" s="113"/>
       <c r="AV82" s="34"/>
       <c r="AX82" s="34"/>
-      <c r="AY82" s="78"/>
+      <c r="AY82" s="113"/>
       <c r="AZ82" s="34"/>
     </row>
     <row r="83" spans="2:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -8982,11 +8982,11 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
-      <c r="M83" s="100"/>
-      <c r="N83" s="101"/>
-      <c r="O83" s="95"/>
-      <c r="P83" s="95"/>
-      <c r="Q83" s="104"/>
+      <c r="M83" s="95"/>
+      <c r="N83" s="97"/>
+      <c r="O83" s="91"/>
+      <c r="P83" s="91"/>
+      <c r="Q83" s="110"/>
       <c r="T83" s="21">
         <v>1</v>
       </c>
@@ -9005,17 +9005,17 @@
       <c r="Y83" s="19">
         <v>21</v>
       </c>
-      <c r="Z83" s="94"/>
-      <c r="AA83" s="94"/>
-      <c r="AB83" s="94"/>
+      <c r="Z83" s="79"/>
+      <c r="AA83" s="79"/>
+      <c r="AB83" s="79"/>
       <c r="AC83" s="6"/>
       <c r="AD83" s="6"/>
       <c r="AE83" s="6"/>
       <c r="AF83" s="6"/>
       <c r="AI83" s="6"/>
-      <c r="AN83" s="78"/>
+      <c r="AN83" s="113"/>
       <c r="AX83" s="34"/>
-      <c r="AY83" s="78"/>
+      <c r="AY83" s="113"/>
       <c r="AZ83" s="34"/>
     </row>
     <row r="84" spans="2:52" x14ac:dyDescent="0.45">
@@ -9028,11 +9028,11 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
-      <c r="M84" s="100"/>
-      <c r="N84" s="101"/>
-      <c r="O84" s="95"/>
-      <c r="P84" s="95"/>
-      <c r="Q84" s="104"/>
+      <c r="M84" s="95"/>
+      <c r="N84" s="97"/>
+      <c r="O84" s="91"/>
+      <c r="P84" s="91"/>
+      <c r="Q84" s="110"/>
       <c r="T84" s="21">
         <v>1</v>
       </c>
@@ -9051,16 +9051,16 @@
       <c r="Y84" s="19">
         <v>22</v>
       </c>
-      <c r="Z84" s="94"/>
-      <c r="AA84" s="94"/>
-      <c r="AB84" s="94"/>
+      <c r="Z84" s="79"/>
+      <c r="AA84" s="79"/>
+      <c r="AB84" s="79"/>
       <c r="AC84" s="6"/>
       <c r="AD84" s="6"/>
       <c r="AE84" s="6"/>
       <c r="AF84" s="6"/>
-      <c r="AN84" s="78"/>
+      <c r="AN84" s="113"/>
       <c r="AX84" s="34"/>
-      <c r="AY84" s="78"/>
+      <c r="AY84" s="113"/>
       <c r="AZ84" s="34"/>
     </row>
     <row r="85" spans="2:52" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9070,11 +9070,11 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
-      <c r="M85" s="102"/>
-      <c r="N85" s="103"/>
-      <c r="O85" s="95"/>
-      <c r="P85" s="95"/>
-      <c r="Q85" s="104"/>
+      <c r="M85" s="98"/>
+      <c r="N85" s="100"/>
+      <c r="O85" s="91"/>
+      <c r="P85" s="91"/>
+      <c r="Q85" s="110"/>
       <c r="T85" s="21">
         <v>1</v>
       </c>
@@ -9093,16 +9093,16 @@
       <c r="Y85" s="19">
         <v>23</v>
       </c>
-      <c r="Z85" s="94"/>
-      <c r="AA85" s="94"/>
-      <c r="AB85" s="94"/>
+      <c r="Z85" s="79"/>
+      <c r="AA85" s="79"/>
+      <c r="AB85" s="79"/>
       <c r="AC85" s="6"/>
       <c r="AD85" s="6"/>
       <c r="AE85" s="6"/>
       <c r="AF85" s="6"/>
-      <c r="AN85" s="79"/>
+      <c r="AN85" s="114"/>
       <c r="AX85" s="34"/>
-      <c r="AY85" s="79"/>
+      <c r="AY85" s="114"/>
       <c r="AZ85" s="34"/>
     </row>
     <row r="86" spans="2:52" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9142,9 +9142,9 @@
       <c r="Y86" s="19">
         <v>24</v>
       </c>
-      <c r="Z86" s="94"/>
-      <c r="AA86" s="94"/>
-      <c r="AB86" s="94"/>
+      <c r="Z86" s="79"/>
+      <c r="AA86" s="79"/>
+      <c r="AB86" s="79"/>
       <c r="AC86" s="6"/>
       <c r="AD86" s="6"/>
       <c r="AE86" s="6"/>
@@ -9192,18 +9192,18 @@
       <c r="Y87" s="19">
         <v>25</v>
       </c>
-      <c r="Z87" s="94"/>
-      <c r="AA87" s="94"/>
-      <c r="AB87" s="94"/>
+      <c r="Z87" s="79"/>
+      <c r="AA87" s="79"/>
+      <c r="AB87" s="79"/>
       <c r="AC87" s="6"/>
       <c r="AD87" s="6"/>
       <c r="AE87" s="6"/>
       <c r="AF87" s="6"/>
-      <c r="AN87" s="77" t="s">
+      <c r="AN87" s="112" t="s">
         <v>124</v>
       </c>
       <c r="AX87" s="34"/>
-      <c r="AY87" s="77" t="s">
+      <c r="AY87" s="112" t="s">
         <v>130</v>
       </c>
       <c r="AZ87" s="34"/>
@@ -9247,16 +9247,16 @@
       <c r="Y88" s="19">
         <v>26</v>
       </c>
-      <c r="Z88" s="94"/>
-      <c r="AA88" s="94"/>
-      <c r="AB88" s="94"/>
+      <c r="Z88" s="79"/>
+      <c r="AA88" s="79"/>
+      <c r="AB88" s="79"/>
       <c r="AC88" s="6"/>
       <c r="AD88" s="6"/>
       <c r="AE88" s="6"/>
       <c r="AF88" s="6"/>
-      <c r="AN88" s="78"/>
+      <c r="AN88" s="113"/>
       <c r="AX88" s="34"/>
-      <c r="AY88" s="78"/>
+      <c r="AY88" s="113"/>
       <c r="AZ88" s="34"/>
     </row>
     <row r="89" spans="2:52" x14ac:dyDescent="0.45">
@@ -9299,16 +9299,16 @@
       <c r="Y89" s="19">
         <v>27</v>
       </c>
-      <c r="Z89" s="94"/>
-      <c r="AA89" s="94"/>
-      <c r="AB89" s="94"/>
+      <c r="Z89" s="79"/>
+      <c r="AA89" s="79"/>
+      <c r="AB89" s="79"/>
       <c r="AC89" s="6"/>
       <c r="AD89" s="6"/>
       <c r="AE89" s="6"/>
       <c r="AF89" s="6"/>
-      <c r="AN89" s="78"/>
+      <c r="AN89" s="113"/>
       <c r="AX89" s="34"/>
-      <c r="AY89" s="78"/>
+      <c r="AY89" s="113"/>
       <c r="AZ89" s="34"/>
     </row>
     <row r="90" spans="2:52" x14ac:dyDescent="0.45">
@@ -9342,16 +9342,16 @@
       <c r="Y90" s="19">
         <v>28</v>
       </c>
-      <c r="Z90" s="94"/>
-      <c r="AA90" s="94"/>
-      <c r="AB90" s="94"/>
+      <c r="Z90" s="79"/>
+      <c r="AA90" s="79"/>
+      <c r="AB90" s="79"/>
       <c r="AC90" s="6"/>
       <c r="AD90" s="6"/>
       <c r="AE90" s="6"/>
       <c r="AF90" s="6"/>
-      <c r="AN90" s="78"/>
+      <c r="AN90" s="113"/>
       <c r="AX90" s="34"/>
-      <c r="AY90" s="78"/>
+      <c r="AY90" s="113"/>
       <c r="AZ90" s="34"/>
     </row>
     <row r="91" spans="2:52" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9385,16 +9385,16 @@
       <c r="Y91" s="19">
         <v>29</v>
       </c>
-      <c r="Z91" s="94"/>
-      <c r="AA91" s="94"/>
-      <c r="AB91" s="94"/>
+      <c r="Z91" s="79"/>
+      <c r="AA91" s="79"/>
+      <c r="AB91" s="79"/>
       <c r="AC91" s="6"/>
       <c r="AD91" s="6"/>
       <c r="AE91" s="6"/>
       <c r="AF91" s="6"/>
-      <c r="AN91" s="79"/>
+      <c r="AN91" s="114"/>
       <c r="AX91" s="34"/>
-      <c r="AY91" s="79"/>
+      <c r="AY91" s="114"/>
       <c r="AZ91" s="34"/>
     </row>
     <row r="92" spans="2:52" x14ac:dyDescent="0.45">
@@ -9428,9 +9428,9 @@
       <c r="Y92" s="19">
         <v>30</v>
       </c>
-      <c r="Z92" s="94"/>
-      <c r="AA92" s="94"/>
-      <c r="AB92" s="94"/>
+      <c r="Z92" s="79"/>
+      <c r="AA92" s="79"/>
+      <c r="AB92" s="79"/>
       <c r="AC92" s="6"/>
       <c r="AD92" s="6"/>
       <c r="AE92" s="6"/>
@@ -9467,11 +9467,11 @@
       <c r="Y93" s="19">
         <v>31</v>
       </c>
-      <c r="Z93" s="94" t="s">
+      <c r="Z93" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="AA93" s="94"/>
-      <c r="AB93" s="94"/>
+      <c r="AA93" s="79"/>
+      <c r="AB93" s="79"/>
       <c r="AC93" s="6"/>
       <c r="AD93" s="6"/>
       <c r="AE93" s="6"/>
@@ -9481,10 +9481,10 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
-      <c r="H94" s="118" t="s">
+      <c r="H94" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="I94" s="118" t="s">
+      <c r="I94" s="83" t="s">
         <v>160</v>
       </c>
       <c r="J94" s="28"/>
@@ -9508,128 +9508,128 @@
       <c r="AG94" s="1"/>
     </row>
     <row r="95" spans="2:52" x14ac:dyDescent="0.45">
-      <c r="B95" s="91" t="s">
+      <c r="B95" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C95" s="91"/>
-      <c r="D95" s="91"/>
-      <c r="E95" s="118" t="s">
+      <c r="C95" s="85"/>
+      <c r="D95" s="85"/>
+      <c r="E95" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="F95" s="118"/>
-      <c r="G95" s="118"/>
-      <c r="H95" s="118"/>
-      <c r="I95" s="118"/>
-      <c r="J95" s="91" t="s">
+      <c r="F95" s="83"/>
+      <c r="G95" s="83"/>
+      <c r="H95" s="83"/>
+      <c r="I95" s="83"/>
+      <c r="J95" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="K95" s="91"/>
-      <c r="L95" s="91" t="s">
+      <c r="K95" s="85"/>
+      <c r="L95" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="M95" s="91"/>
-      <c r="N95" s="91" t="s">
+      <c r="M95" s="85"/>
+      <c r="N95" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="O95" s="91"/>
-      <c r="P95" s="91" t="s">
+      <c r="O95" s="85"/>
+      <c r="P95" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="Q95" s="91"/>
-      <c r="R95" s="91" t="s">
+      <c r="Q95" s="85"/>
+      <c r="R95" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S95" s="91"/>
-      <c r="T95" s="91"/>
-      <c r="U95" s="91"/>
-      <c r="V95" s="91"/>
-      <c r="W95" s="91" t="s">
+      <c r="S95" s="85"/>
+      <c r="T95" s="85"/>
+      <c r="U95" s="85"/>
+      <c r="V95" s="85"/>
+      <c r="W95" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="X95" s="91"/>
-      <c r="Y95" s="91" t="s">
+      <c r="X95" s="85"/>
+      <c r="Y95" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="Z95" s="91"/>
-      <c r="AA95" s="91" t="s">
+      <c r="Z95" s="85"/>
+      <c r="AA95" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="AB95" s="91"/>
-      <c r="AC95" s="91" t="s">
+      <c r="AB95" s="85"/>
+      <c r="AC95" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="AD95" s="91"/>
-      <c r="AE95" s="91"/>
-      <c r="AF95" s="91"/>
-      <c r="AG95" s="91"/>
+      <c r="AD95" s="85"/>
+      <c r="AE95" s="85"/>
+      <c r="AF95" s="85"/>
+      <c r="AG95" s="85"/>
     </row>
     <row r="96" spans="2:52" x14ac:dyDescent="0.45">
-      <c r="B96" s="91"/>
-      <c r="C96" s="91"/>
-      <c r="D96" s="91"/>
-      <c r="E96" s="118"/>
-      <c r="F96" s="118"/>
-      <c r="G96" s="118"/>
-      <c r="H96" s="118"/>
-      <c r="I96" s="118"/>
-      <c r="J96" s="91"/>
-      <c r="K96" s="91"/>
-      <c r="L96" s="91"/>
-      <c r="M96" s="91"/>
-      <c r="N96" s="91"/>
-      <c r="O96" s="91"/>
-      <c r="P96" s="91"/>
-      <c r="Q96" s="91"/>
-      <c r="R96" s="91"/>
-      <c r="S96" s="91"/>
-      <c r="T96" s="91"/>
-      <c r="U96" s="91"/>
-      <c r="V96" s="91"/>
-      <c r="W96" s="91"/>
-      <c r="X96" s="91"/>
-      <c r="Y96" s="91"/>
-      <c r="Z96" s="91"/>
-      <c r="AA96" s="91"/>
-      <c r="AB96" s="91"/>
-      <c r="AC96" s="91"/>
-      <c r="AD96" s="91"/>
-      <c r="AE96" s="91"/>
-      <c r="AF96" s="91"/>
-      <c r="AG96" s="91"/>
+      <c r="B96" s="85"/>
+      <c r="C96" s="85"/>
+      <c r="D96" s="85"/>
+      <c r="E96" s="83"/>
+      <c r="F96" s="83"/>
+      <c r="G96" s="83"/>
+      <c r="H96" s="83"/>
+      <c r="I96" s="83"/>
+      <c r="J96" s="85"/>
+      <c r="K96" s="85"/>
+      <c r="L96" s="85"/>
+      <c r="M96" s="85"/>
+      <c r="N96" s="85"/>
+      <c r="O96" s="85"/>
+      <c r="P96" s="85"/>
+      <c r="Q96" s="85"/>
+      <c r="R96" s="85"/>
+      <c r="S96" s="85"/>
+      <c r="T96" s="85"/>
+      <c r="U96" s="85"/>
+      <c r="V96" s="85"/>
+      <c r="W96" s="85"/>
+      <c r="X96" s="85"/>
+      <c r="Y96" s="85"/>
+      <c r="Z96" s="85"/>
+      <c r="AA96" s="85"/>
+      <c r="AB96" s="85"/>
+      <c r="AC96" s="85"/>
+      <c r="AD96" s="85"/>
+      <c r="AE96" s="85"/>
+      <c r="AF96" s="85"/>
+      <c r="AG96" s="85"/>
     </row>
     <row r="97" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="B97" s="92"/>
-      <c r="C97" s="92"/>
-      <c r="D97" s="92"/>
-      <c r="E97" s="92"/>
-      <c r="F97" s="92"/>
-      <c r="G97" s="92"/>
-      <c r="H97" s="92"/>
-      <c r="I97" s="92"/>
-      <c r="J97" s="92"/>
-      <c r="K97" s="92"/>
-      <c r="L97" s="92"/>
-      <c r="M97" s="92"/>
-      <c r="N97" s="92"/>
-      <c r="O97" s="92"/>
-      <c r="P97" s="92"/>
-      <c r="Q97" s="92"/>
-      <c r="R97" s="92"/>
-      <c r="S97" s="92"/>
-      <c r="T97" s="92"/>
-      <c r="U97" s="92"/>
-      <c r="V97" s="92"/>
-      <c r="W97" s="92"/>
-      <c r="X97" s="92"/>
-      <c r="Y97" s="92"/>
-      <c r="Z97" s="92"/>
-      <c r="AA97" s="92"/>
-      <c r="AB97" s="92"/>
-      <c r="AC97" s="92"/>
-      <c r="AD97" s="92"/>
-      <c r="AE97" s="92"/>
-      <c r="AF97" s="92"/>
-      <c r="AG97" s="92"/>
+      <c r="B97" s="84"/>
+      <c r="C97" s="84"/>
+      <c r="D97" s="84"/>
+      <c r="E97" s="84"/>
+      <c r="F97" s="84"/>
+      <c r="G97" s="84"/>
+      <c r="H97" s="84"/>
+      <c r="I97" s="84"/>
+      <c r="J97" s="84"/>
+      <c r="K97" s="84"/>
+      <c r="L97" s="84"/>
+      <c r="M97" s="84"/>
+      <c r="N97" s="84"/>
+      <c r="O97" s="84"/>
+      <c r="P97" s="84"/>
+      <c r="Q97" s="84"/>
+      <c r="R97" s="84"/>
+      <c r="S97" s="84"/>
+      <c r="T97" s="84"/>
+      <c r="U97" s="84"/>
+      <c r="V97" s="84"/>
+      <c r="W97" s="84"/>
+      <c r="X97" s="84"/>
+      <c r="Y97" s="84"/>
+      <c r="Z97" s="84"/>
+      <c r="AA97" s="84"/>
+      <c r="AB97" s="84"/>
+      <c r="AC97" s="84"/>
+      <c r="AD97" s="84"/>
+      <c r="AE97" s="84"/>
+      <c r="AF97" s="84"/>
+      <c r="AG97" s="84"/>
     </row>
     <row r="98" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B98" s="18">
@@ -9736,45 +9736,45 @@
       <c r="B99" s="36">
         <v>1</v>
       </c>
-      <c r="C99" s="115" t="s">
+      <c r="C99" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="D99" s="116"/>
-      <c r="E99" s="116"/>
-      <c r="F99" s="116"/>
-      <c r="G99" s="116"/>
-      <c r="H99" s="116"/>
-      <c r="I99" s="116"/>
-      <c r="J99" s="116"/>
-      <c r="K99" s="116"/>
-      <c r="L99" s="116"/>
-      <c r="M99" s="116"/>
-      <c r="N99" s="116"/>
-      <c r="O99" s="116"/>
-      <c r="P99" s="116"/>
-      <c r="Q99" s="116"/>
-      <c r="R99" s="116"/>
-      <c r="S99" s="116"/>
-      <c r="T99" s="116"/>
-      <c r="U99" s="116"/>
-      <c r="V99" s="116"/>
-      <c r="W99" s="116"/>
-      <c r="X99" s="116"/>
-      <c r="Y99" s="116"/>
-      <c r="Z99" s="116"/>
-      <c r="AA99" s="116"/>
-      <c r="AB99" s="116"/>
-      <c r="AC99" s="116"/>
-      <c r="AD99" s="116"/>
-      <c r="AE99" s="116"/>
-      <c r="AF99" s="116"/>
-      <c r="AG99" s="117"/>
+      <c r="D99" s="81"/>
+      <c r="E99" s="81"/>
+      <c r="F99" s="81"/>
+      <c r="G99" s="81"/>
+      <c r="H99" s="81"/>
+      <c r="I99" s="81"/>
+      <c r="J99" s="81"/>
+      <c r="K99" s="81"/>
+      <c r="L99" s="81"/>
+      <c r="M99" s="81"/>
+      <c r="N99" s="81"/>
+      <c r="O99" s="81"/>
+      <c r="P99" s="81"/>
+      <c r="Q99" s="81"/>
+      <c r="R99" s="81"/>
+      <c r="S99" s="81"/>
+      <c r="T99" s="81"/>
+      <c r="U99" s="81"/>
+      <c r="V99" s="81"/>
+      <c r="W99" s="81"/>
+      <c r="X99" s="81"/>
+      <c r="Y99" s="81"/>
+      <c r="Z99" s="81"/>
+      <c r="AA99" s="81"/>
+      <c r="AB99" s="81"/>
+      <c r="AC99" s="81"/>
+      <c r="AD99" s="81"/>
+      <c r="AE99" s="81"/>
+      <c r="AF99" s="81"/>
+      <c r="AG99" s="82"/>
       <c r="AH99" s="6"/>
-      <c r="AI99" s="76" t="s">
+      <c r="AI99" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="AJ99" s="76"/>
-      <c r="AK99" s="76"/>
+      <c r="AJ99" s="78"/>
+      <c r="AK99" s="78"/>
     </row>
     <row r="100" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A100" s="35" t="s">
@@ -9825,18 +9825,18 @@
       <c r="Z100" s="37"/>
       <c r="AA100" s="42"/>
       <c r="AB100" s="37"/>
-      <c r="AC100" s="120" t="s">
+      <c r="AC100" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="AD100" s="116"/>
-      <c r="AE100" s="116"/>
-      <c r="AF100" s="116"/>
-      <c r="AG100" s="117"/>
-      <c r="AI100" s="76" t="s">
+      <c r="AD100" s="81"/>
+      <c r="AE100" s="81"/>
+      <c r="AF100" s="81"/>
+      <c r="AG100" s="82"/>
+      <c r="AI100" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="AJ100" s="76"/>
-      <c r="AK100" s="76"/>
+      <c r="AJ100" s="78"/>
+      <c r="AK100" s="78"/>
     </row>
     <row r="101" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A101" s="35" t="s">
@@ -9900,11 +9900,11 @@
       <c r="AE101" s="40"/>
       <c r="AF101" s="40"/>
       <c r="AG101" s="41"/>
-      <c r="AI101" s="76" t="s">
+      <c r="AI101" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="AJ101" s="76"/>
-      <c r="AK101" s="76"/>
+      <c r="AJ101" s="78"/>
+      <c r="AK101" s="78"/>
     </row>
     <row r="102" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A102" s="35" t="s">
@@ -9976,11 +9976,11 @@
       <c r="AE102" s="40"/>
       <c r="AF102" s="40"/>
       <c r="AG102" s="41"/>
-      <c r="AI102" s="76" t="s">
+      <c r="AI102" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="AJ102" s="76"/>
-      <c r="AK102" s="76"/>
+      <c r="AJ102" s="78"/>
+      <c r="AK102" s="78"/>
     </row>
     <row r="103" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A103" s="35" t="s">
@@ -10030,11 +10030,11 @@
       <c r="AE103" s="40"/>
       <c r="AF103" s="40"/>
       <c r="AG103" s="41"/>
-      <c r="AI103" s="76" t="s">
+      <c r="AI103" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="AJ103" s="76"/>
-      <c r="AK103" s="76"/>
+      <c r="AJ103" s="78"/>
+      <c r="AK103" s="78"/>
     </row>
     <row r="104" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A104" s="35" t="s">
@@ -10100,11 +10100,11 @@
       <c r="AE104" s="40"/>
       <c r="AF104" s="40"/>
       <c r="AG104" s="41"/>
-      <c r="AI104" s="76" t="s">
+      <c r="AI104" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="AJ104" s="76"/>
-      <c r="AK104" s="76"/>
+      <c r="AJ104" s="78"/>
+      <c r="AK104" s="78"/>
     </row>
     <row r="105" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A105" s="35" t="s">
@@ -10138,29 +10138,29 @@
       <c r="O105" s="37"/>
       <c r="P105" s="42"/>
       <c r="Q105" s="37"/>
-      <c r="R105" s="120" t="s">
+      <c r="R105" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="S105" s="116"/>
-      <c r="T105" s="116"/>
-      <c r="U105" s="116"/>
-      <c r="V105" s="116"/>
-      <c r="W105" s="116"/>
-      <c r="X105" s="116"/>
-      <c r="Y105" s="116"/>
-      <c r="Z105" s="116"/>
-      <c r="AA105" s="116"/>
-      <c r="AB105" s="116"/>
-      <c r="AC105" s="116"/>
-      <c r="AD105" s="116"/>
-      <c r="AE105" s="116"/>
-      <c r="AF105" s="116"/>
-      <c r="AG105" s="117"/>
-      <c r="AI105" s="76" t="s">
+      <c r="S105" s="81"/>
+      <c r="T105" s="81"/>
+      <c r="U105" s="81"/>
+      <c r="V105" s="81"/>
+      <c r="W105" s="81"/>
+      <c r="X105" s="81"/>
+      <c r="Y105" s="81"/>
+      <c r="Z105" s="81"/>
+      <c r="AA105" s="81"/>
+      <c r="AB105" s="81"/>
+      <c r="AC105" s="81"/>
+      <c r="AD105" s="81"/>
+      <c r="AE105" s="81"/>
+      <c r="AF105" s="81"/>
+      <c r="AG105" s="82"/>
+      <c r="AI105" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="AJ105" s="76"/>
-      <c r="AK105" s="76"/>
+      <c r="AJ105" s="78"/>
+      <c r="AK105" s="78"/>
     </row>
     <row r="106" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A106" s="35" t="s">
@@ -10234,17 +10234,17 @@
       <c r="AE106" s="40"/>
       <c r="AF106" s="40"/>
       <c r="AG106" s="41"/>
-      <c r="AI106" s="76" t="s">
+      <c r="AI106" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="AJ106" s="76"/>
-      <c r="AK106" s="76"/>
-      <c r="AL106" s="84" t="s">
+      <c r="AJ106" s="78"/>
+      <c r="AK106" s="78"/>
+      <c r="AL106" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="AM106" s="84"/>
-      <c r="AN106" s="84"/>
-      <c r="AO106" s="84"/>
+      <c r="AM106" s="125"/>
+      <c r="AN106" s="125"/>
+      <c r="AO106" s="125"/>
     </row>
     <row r="107" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A107" s="35" t="s">
@@ -10312,17 +10312,17 @@
       <c r="AE107" s="40"/>
       <c r="AF107" s="40"/>
       <c r="AG107" s="41"/>
-      <c r="AI107" s="76" t="s">
+      <c r="AI107" s="78" t="s">
         <v>173</v>
       </c>
-      <c r="AJ107" s="76"/>
-      <c r="AK107" s="76"/>
-      <c r="AL107" s="84" t="s">
+      <c r="AJ107" s="78"/>
+      <c r="AK107" s="78"/>
+      <c r="AL107" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="AM107" s="84"/>
-      <c r="AN107" s="84"/>
-      <c r="AO107" s="84"/>
+      <c r="AM107" s="125"/>
+      <c r="AN107" s="125"/>
+      <c r="AO107" s="125"/>
     </row>
     <row r="108" spans="1:41" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A108" s="35" t="s">
@@ -10374,11 +10374,11 @@
       <c r="AE108" s="40"/>
       <c r="AF108" s="40"/>
       <c r="AG108" s="41"/>
-      <c r="AI108" s="76" t="s">
+      <c r="AI108" s="78" t="s">
         <v>154</v>
       </c>
-      <c r="AJ108" s="76"/>
-      <c r="AK108" s="76"/>
+      <c r="AJ108" s="78"/>
+      <c r="AK108" s="78"/>
     </row>
     <row r="109" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A109" s="35" t="s">
@@ -10426,11 +10426,11 @@
       <c r="AE109" s="40"/>
       <c r="AF109" s="40"/>
       <c r="AG109" s="41"/>
-      <c r="AI109" s="76" t="s">
+      <c r="AI109" s="78" t="s">
         <v>155</v>
       </c>
-      <c r="AJ109" s="76"/>
-      <c r="AK109" s="76"/>
+      <c r="AJ109" s="78"/>
+      <c r="AK109" s="78"/>
     </row>
     <row r="110" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A110" s="35" t="s">
@@ -10492,11 +10492,11 @@
       <c r="AE110" s="40"/>
       <c r="AF110" s="40"/>
       <c r="AG110" s="41"/>
-      <c r="AI110" s="76" t="s">
+      <c r="AI110" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="AJ110" s="76"/>
-      <c r="AK110" s="76"/>
+      <c r="AJ110" s="78"/>
+      <c r="AK110" s="78"/>
     </row>
     <row r="111" spans="1:41" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A111" s="35" t="s">
@@ -10544,11 +10544,11 @@
       <c r="AE111" s="40"/>
       <c r="AF111" s="40"/>
       <c r="AG111" s="41"/>
-      <c r="AI111" s="76" t="s">
+      <c r="AI111" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="AJ111" s="76"/>
-      <c r="AK111" s="76"/>
+      <c r="AJ111" s="78"/>
+      <c r="AK111" s="78"/>
       <c r="AL111" s="6" t="s">
         <v>114</v>
       </c>
@@ -10619,11 +10619,11 @@
       <c r="AE112" s="40"/>
       <c r="AF112" s="40"/>
       <c r="AG112" s="41"/>
-      <c r="AI112" s="76" t="s">
+      <c r="AI112" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="AJ112" s="76"/>
-      <c r="AK112" s="76"/>
+      <c r="AJ112" s="78"/>
+      <c r="AK112" s="78"/>
     </row>
     <row r="113" spans="1:44" x14ac:dyDescent="0.45">
       <c r="A113" s="30"/>
@@ -10650,11 +10650,11 @@
       <c r="D114" s="27">
         <v>1</v>
       </c>
-      <c r="E114" s="124"/>
-      <c r="F114" s="125"/>
-      <c r="G114" s="125"/>
-      <c r="H114" s="125"/>
-      <c r="I114" s="125"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="77"/>
+      <c r="G114" s="77"/>
+      <c r="H114" s="77"/>
+      <c r="I114" s="77"/>
       <c r="J114" s="71"/>
       <c r="K114" s="71"/>
       <c r="L114" s="71"/>
@@ -10679,11 +10679,11 @@
       <c r="AE114" s="71"/>
       <c r="AF114" s="71"/>
       <c r="AG114" s="72"/>
-      <c r="AI114" s="76" t="s">
+      <c r="AI114" s="78" t="s">
         <v>176</v>
       </c>
-      <c r="AJ114" s="76"/>
-      <c r="AK114" s="76"/>
+      <c r="AJ114" s="78"/>
+      <c r="AK114" s="78"/>
     </row>
     <row r="115" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E115" s="28"/>
@@ -11291,41 +11291,41 @@
       <c r="I168" s="6"/>
     </row>
     <row r="178" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A178" s="119" t="s">
+      <c r="A178" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="B178" s="119"/>
-      <c r="C178" s="119"/>
-      <c r="D178" s="119"/>
-      <c r="E178" s="119"/>
-      <c r="F178" s="119"/>
-      <c r="G178" s="119"/>
-      <c r="H178" s="119"/>
-      <c r="I178" s="119"/>
-      <c r="J178" s="119"/>
-      <c r="K178" s="119"/>
-      <c r="L178" s="119"/>
-      <c r="M178" s="119"/>
-      <c r="N178" s="119"/>
-      <c r="O178" s="119"/>
-      <c r="P178" s="119"/>
-      <c r="Q178" s="119"/>
-      <c r="R178" s="119"/>
-      <c r="S178" s="119"/>
-      <c r="T178" s="119"/>
-      <c r="U178" s="119"/>
-      <c r="V178" s="119"/>
-      <c r="W178" s="119"/>
-      <c r="X178" s="119"/>
-      <c r="Y178" s="119"/>
-      <c r="Z178" s="119"/>
-      <c r="AA178" s="119"/>
-      <c r="AB178" s="119"/>
-      <c r="AC178" s="119"/>
-      <c r="AD178" s="119"/>
-      <c r="AE178" s="119"/>
-      <c r="AF178" s="119"/>
-      <c r="AG178" s="119"/>
+      <c r="B178" s="86"/>
+      <c r="C178" s="86"/>
+      <c r="D178" s="86"/>
+      <c r="E178" s="86"/>
+      <c r="F178" s="86"/>
+      <c r="G178" s="86"/>
+      <c r="H178" s="86"/>
+      <c r="I178" s="86"/>
+      <c r="J178" s="86"/>
+      <c r="K178" s="86"/>
+      <c r="L178" s="86"/>
+      <c r="M178" s="86"/>
+      <c r="N178" s="86"/>
+      <c r="O178" s="86"/>
+      <c r="P178" s="86"/>
+      <c r="Q178" s="86"/>
+      <c r="R178" s="86"/>
+      <c r="S178" s="86"/>
+      <c r="T178" s="86"/>
+      <c r="U178" s="86"/>
+      <c r="V178" s="86"/>
+      <c r="W178" s="86"/>
+      <c r="X178" s="86"/>
+      <c r="Y178" s="86"/>
+      <c r="Z178" s="86"/>
+      <c r="AA178" s="86"/>
+      <c r="AB178" s="86"/>
+      <c r="AC178" s="86"/>
+      <c r="AD178" s="86"/>
+      <c r="AE178" s="86"/>
+      <c r="AF178" s="86"/>
+      <c r="AG178" s="86"/>
       <c r="AH178" s="29"/>
       <c r="AI178" s="29"/>
     </row>
@@ -11431,100 +11431,210 @@
       <c r="A184" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B184" s="106" t="s">
+      <c r="B184" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="C184" s="107"/>
-      <c r="D184" s="107"/>
-      <c r="E184" s="107"/>
-      <c r="F184" s="107"/>
-      <c r="G184" s="107"/>
-      <c r="H184" s="107"/>
-      <c r="I184" s="107"/>
-      <c r="J184" s="107"/>
-      <c r="K184" s="107"/>
-      <c r="L184" s="107"/>
-      <c r="M184" s="107"/>
-      <c r="N184" s="107"/>
-      <c r="O184" s="107"/>
-      <c r="P184" s="107"/>
-      <c r="Q184" s="107"/>
-      <c r="R184" s="107"/>
-      <c r="S184" s="107"/>
-      <c r="T184" s="107"/>
-      <c r="U184" s="107"/>
-      <c r="V184" s="107"/>
-      <c r="W184" s="107"/>
-      <c r="X184" s="107"/>
-      <c r="Y184" s="107"/>
-      <c r="Z184" s="107"/>
-      <c r="AA184" s="107"/>
-      <c r="AB184" s="107"/>
-      <c r="AC184" s="107"/>
-      <c r="AD184" s="107"/>
-      <c r="AE184" s="107"/>
-      <c r="AF184" s="107"/>
-      <c r="AG184" s="108"/>
+      <c r="C184" s="88"/>
+      <c r="D184" s="88"/>
+      <c r="E184" s="88"/>
+      <c r="F184" s="88"/>
+      <c r="G184" s="88"/>
+      <c r="H184" s="88"/>
+      <c r="I184" s="88"/>
+      <c r="J184" s="88"/>
+      <c r="K184" s="88"/>
+      <c r="L184" s="88"/>
+      <c r="M184" s="88"/>
+      <c r="N184" s="88"/>
+      <c r="O184" s="88"/>
+      <c r="P184" s="88"/>
+      <c r="Q184" s="88"/>
+      <c r="R184" s="88"/>
+      <c r="S184" s="88"/>
+      <c r="T184" s="88"/>
+      <c r="U184" s="88"/>
+      <c r="V184" s="88"/>
+      <c r="W184" s="88"/>
+      <c r="X184" s="88"/>
+      <c r="Y184" s="88"/>
+      <c r="Z184" s="88"/>
+      <c r="AA184" s="88"/>
+      <c r="AB184" s="88"/>
+      <c r="AC184" s="88"/>
+      <c r="AD184" s="88"/>
+      <c r="AE184" s="88"/>
+      <c r="AF184" s="88"/>
+      <c r="AG184" s="89"/>
     </row>
     <row r="186" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A186" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B186" s="106" t="s">
+      <c r="B186" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="C186" s="107"/>
-      <c r="D186" s="107"/>
-      <c r="E186" s="107"/>
-      <c r="F186" s="107"/>
-      <c r="G186" s="107"/>
-      <c r="H186" s="107"/>
-      <c r="I186" s="107"/>
-      <c r="J186" s="107"/>
-      <c r="K186" s="107"/>
-      <c r="L186" s="107"/>
-      <c r="M186" s="107"/>
-      <c r="N186" s="107"/>
-      <c r="O186" s="107"/>
-      <c r="P186" s="107"/>
-      <c r="Q186" s="108"/>
-      <c r="R186" s="106" t="s">
+      <c r="C186" s="88"/>
+      <c r="D186" s="88"/>
+      <c r="E186" s="88"/>
+      <c r="F186" s="88"/>
+      <c r="G186" s="88"/>
+      <c r="H186" s="88"/>
+      <c r="I186" s="88"/>
+      <c r="J186" s="88"/>
+      <c r="K186" s="88"/>
+      <c r="L186" s="88"/>
+      <c r="M186" s="88"/>
+      <c r="N186" s="88"/>
+      <c r="O186" s="88"/>
+      <c r="P186" s="88"/>
+      <c r="Q186" s="89"/>
+      <c r="R186" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="S186" s="107"/>
-      <c r="T186" s="107"/>
-      <c r="U186" s="107"/>
-      <c r="V186" s="107"/>
-      <c r="W186" s="107"/>
-      <c r="X186" s="107"/>
-      <c r="Y186" s="107"/>
-      <c r="Z186" s="107"/>
-      <c r="AA186" s="107"/>
-      <c r="AB186" s="107"/>
-      <c r="AC186" s="107"/>
-      <c r="AD186" s="107"/>
-      <c r="AE186" s="107"/>
-      <c r="AF186" s="107"/>
-      <c r="AG186" s="108"/>
+      <c r="S186" s="88"/>
+      <c r="T186" s="88"/>
+      <c r="U186" s="88"/>
+      <c r="V186" s="88"/>
+      <c r="W186" s="88"/>
+      <c r="X186" s="88"/>
+      <c r="Y186" s="88"/>
+      <c r="Z186" s="88"/>
+      <c r="AA186" s="88"/>
+      <c r="AB186" s="88"/>
+      <c r="AC186" s="88"/>
+      <c r="AD186" s="88"/>
+      <c r="AE186" s="88"/>
+      <c r="AF186" s="88"/>
+      <c r="AG186" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="168">
-    <mergeCell ref="AI114:AK114"/>
-    <mergeCell ref="Z93:AB93"/>
-    <mergeCell ref="R105:AG105"/>
-    <mergeCell ref="H94:H97"/>
-    <mergeCell ref="I94:I97"/>
-    <mergeCell ref="B95:D97"/>
-    <mergeCell ref="E95:G97"/>
-    <mergeCell ref="J95:K97"/>
-    <mergeCell ref="L95:M97"/>
-    <mergeCell ref="N95:O97"/>
-    <mergeCell ref="P95:Q97"/>
-    <mergeCell ref="R95:V97"/>
-    <mergeCell ref="W95:X97"/>
-    <mergeCell ref="Y95:Z97"/>
-    <mergeCell ref="AA95:AB97"/>
-    <mergeCell ref="AC95:AG97"/>
+    <mergeCell ref="AN60:AN72"/>
+    <mergeCell ref="AN81:AN85"/>
+    <mergeCell ref="AN87:AN91"/>
+    <mergeCell ref="AQ71:AR71"/>
+    <mergeCell ref="AN78:AO78"/>
+    <mergeCell ref="AI107:AK107"/>
+    <mergeCell ref="AI108:AK108"/>
+    <mergeCell ref="AI109:AK109"/>
+    <mergeCell ref="AI110:AK110"/>
+    <mergeCell ref="AI102:AK102"/>
+    <mergeCell ref="AI103:AK103"/>
+    <mergeCell ref="AI104:AK104"/>
+    <mergeCell ref="AI105:AK105"/>
+    <mergeCell ref="AI106:AK106"/>
+    <mergeCell ref="AL106:AO106"/>
+    <mergeCell ref="AL107:AO107"/>
+    <mergeCell ref="AI100:AK100"/>
+    <mergeCell ref="AI101:AK101"/>
+    <mergeCell ref="AY60:AY72"/>
+    <mergeCell ref="AX78:AY78"/>
+    <mergeCell ref="AY81:AY85"/>
+    <mergeCell ref="AY87:AY91"/>
+    <mergeCell ref="AQ78:AR81"/>
+    <mergeCell ref="AU71:AV71"/>
+    <mergeCell ref="AQ61:AR64"/>
+    <mergeCell ref="B57:D59"/>
+    <mergeCell ref="P57:Q59"/>
+    <mergeCell ref="Q71:Q76"/>
+    <mergeCell ref="Z78:AB78"/>
+    <mergeCell ref="Z79:AB79"/>
+    <mergeCell ref="Z80:AB80"/>
+    <mergeCell ref="Z81:AB81"/>
+    <mergeCell ref="Z82:AB82"/>
+    <mergeCell ref="Z73:AB73"/>
+    <mergeCell ref="Z74:AB74"/>
+    <mergeCell ref="Z75:AB75"/>
+    <mergeCell ref="Z76:AB76"/>
+    <mergeCell ref="Z77:AB77"/>
+    <mergeCell ref="Z88:AB88"/>
+    <mergeCell ref="Z89:AB89"/>
+    <mergeCell ref="Z90:AB90"/>
+    <mergeCell ref="K62:K65"/>
+    <mergeCell ref="AJ11:AQ11"/>
+    <mergeCell ref="AJ12:AQ12"/>
+    <mergeCell ref="AJ13:AQ13"/>
+    <mergeCell ref="B77:C79"/>
+    <mergeCell ref="O82:O85"/>
+    <mergeCell ref="P82:P85"/>
+    <mergeCell ref="Q82:Q85"/>
+    <mergeCell ref="M82:N85"/>
+    <mergeCell ref="M62:N65"/>
+    <mergeCell ref="M71:N76"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="P62:P65"/>
+    <mergeCell ref="Q62:Q65"/>
+    <mergeCell ref="Z66:AB66"/>
+    <mergeCell ref="Z67:AB67"/>
+    <mergeCell ref="Z68:AB68"/>
+    <mergeCell ref="Z69:AB69"/>
+    <mergeCell ref="Z70:AB70"/>
+    <mergeCell ref="Z71:AB71"/>
+    <mergeCell ref="Z72:AB72"/>
+    <mergeCell ref="C50:AG50"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="AJ19:AQ19"/>
+    <mergeCell ref="AJ20:AQ20"/>
+    <mergeCell ref="AJ21:AQ21"/>
+    <mergeCell ref="AJ22:AQ22"/>
+    <mergeCell ref="AJ28:AQ28"/>
+    <mergeCell ref="AJ14:AQ14"/>
+    <mergeCell ref="AJ15:AQ15"/>
+    <mergeCell ref="AJ16:AQ16"/>
+    <mergeCell ref="AJ17:AQ17"/>
+    <mergeCell ref="AJ18:AQ18"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="AJ3:AQ3"/>
+    <mergeCell ref="AJ4:AQ4"/>
+    <mergeCell ref="AJ5:AQ5"/>
+    <mergeCell ref="AJ6:AQ6"/>
+    <mergeCell ref="AJ7:AQ7"/>
+    <mergeCell ref="AJ8:AQ8"/>
+    <mergeCell ref="AJ9:AQ9"/>
+    <mergeCell ref="AJ10:AQ10"/>
+    <mergeCell ref="AJ29:AQ29"/>
+    <mergeCell ref="AJ30:AQ30"/>
+    <mergeCell ref="AJ31:AQ31"/>
+    <mergeCell ref="AJ32:AQ32"/>
+    <mergeCell ref="AJ33:AQ33"/>
+    <mergeCell ref="AJ44:AQ44"/>
+    <mergeCell ref="AJ55:AN55"/>
+    <mergeCell ref="AI99:AK99"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="AJ34:AQ34"/>
+    <mergeCell ref="AJ35:AQ35"/>
+    <mergeCell ref="AJ36:AQ36"/>
+    <mergeCell ref="AJ37:AQ37"/>
+    <mergeCell ref="Z91:AB91"/>
+    <mergeCell ref="Z87:AB87"/>
+    <mergeCell ref="C99:AG99"/>
+    <mergeCell ref="Z92:AB92"/>
+    <mergeCell ref="Z83:AB83"/>
+    <mergeCell ref="Z84:AB84"/>
+    <mergeCell ref="Z85:AB85"/>
+    <mergeCell ref="Z86:AB86"/>
+    <mergeCell ref="R55:AG55"/>
+    <mergeCell ref="P71:P76"/>
+    <mergeCell ref="AA57:AB59"/>
+    <mergeCell ref="W57:X59"/>
+    <mergeCell ref="AC57:AG59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="E57:G59"/>
+    <mergeCell ref="Y57:Z59"/>
+    <mergeCell ref="AJ38:AQ38"/>
+    <mergeCell ref="AJ39:AQ39"/>
+    <mergeCell ref="AJ40:AQ40"/>
+    <mergeCell ref="AJ41:AQ41"/>
+    <mergeCell ref="AJ42:AQ42"/>
+    <mergeCell ref="AJ43:AQ43"/>
+    <mergeCell ref="A47:AI47"/>
+    <mergeCell ref="B52:D54"/>
+    <mergeCell ref="J52:K54"/>
+    <mergeCell ref="L52:M54"/>
+    <mergeCell ref="N52:O54"/>
+    <mergeCell ref="P52:Q54"/>
     <mergeCell ref="A178:AG178"/>
     <mergeCell ref="B184:AG184"/>
     <mergeCell ref="R186:AG186"/>
@@ -11549,134 +11659,24 @@
     <mergeCell ref="J57:K59"/>
     <mergeCell ref="L57:M59"/>
     <mergeCell ref="N57:O59"/>
-    <mergeCell ref="W57:X59"/>
-    <mergeCell ref="AC57:AG59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="E57:G59"/>
-    <mergeCell ref="Y57:Z59"/>
-    <mergeCell ref="AJ38:AQ38"/>
-    <mergeCell ref="AJ39:AQ39"/>
-    <mergeCell ref="AJ40:AQ40"/>
-    <mergeCell ref="AJ41:AQ41"/>
-    <mergeCell ref="AJ42:AQ42"/>
-    <mergeCell ref="AJ43:AQ43"/>
-    <mergeCell ref="A47:AI47"/>
-    <mergeCell ref="B52:D54"/>
-    <mergeCell ref="J52:K54"/>
-    <mergeCell ref="L52:M54"/>
-    <mergeCell ref="N52:O54"/>
-    <mergeCell ref="P52:Q54"/>
-    <mergeCell ref="AJ29:AQ29"/>
-    <mergeCell ref="AJ30:AQ30"/>
-    <mergeCell ref="AJ31:AQ31"/>
-    <mergeCell ref="AJ32:AQ32"/>
-    <mergeCell ref="AJ33:AQ33"/>
-    <mergeCell ref="AJ44:AQ44"/>
-    <mergeCell ref="AJ55:AN55"/>
-    <mergeCell ref="AI99:AK99"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="AJ34:AQ34"/>
-    <mergeCell ref="AJ35:AQ35"/>
-    <mergeCell ref="AJ36:AQ36"/>
-    <mergeCell ref="AJ37:AQ37"/>
-    <mergeCell ref="Z91:AB91"/>
-    <mergeCell ref="Z87:AB87"/>
-    <mergeCell ref="C99:AG99"/>
-    <mergeCell ref="Z92:AB92"/>
-    <mergeCell ref="Z83:AB83"/>
-    <mergeCell ref="Z84:AB84"/>
-    <mergeCell ref="Z85:AB85"/>
-    <mergeCell ref="Z86:AB86"/>
-    <mergeCell ref="R55:AG55"/>
-    <mergeCell ref="P71:P76"/>
-    <mergeCell ref="AA57:AB59"/>
-    <mergeCell ref="AJ2:AQ2"/>
-    <mergeCell ref="AJ3:AQ3"/>
-    <mergeCell ref="AJ4:AQ4"/>
-    <mergeCell ref="AJ5:AQ5"/>
-    <mergeCell ref="AJ6:AQ6"/>
-    <mergeCell ref="AJ7:AQ7"/>
-    <mergeCell ref="AJ8:AQ8"/>
-    <mergeCell ref="AJ9:AQ9"/>
-    <mergeCell ref="AJ10:AQ10"/>
-    <mergeCell ref="AJ19:AQ19"/>
-    <mergeCell ref="AJ20:AQ20"/>
-    <mergeCell ref="AJ21:AQ21"/>
-    <mergeCell ref="AJ22:AQ22"/>
-    <mergeCell ref="AJ28:AQ28"/>
-    <mergeCell ref="AJ14:AQ14"/>
-    <mergeCell ref="AJ15:AQ15"/>
-    <mergeCell ref="AJ16:AQ16"/>
-    <mergeCell ref="AJ17:AQ17"/>
-    <mergeCell ref="AJ18:AQ18"/>
-    <mergeCell ref="AJ11:AQ11"/>
-    <mergeCell ref="AJ12:AQ12"/>
-    <mergeCell ref="AJ13:AQ13"/>
-    <mergeCell ref="B77:C79"/>
-    <mergeCell ref="O82:O85"/>
-    <mergeCell ref="P82:P85"/>
-    <mergeCell ref="Q82:Q85"/>
-    <mergeCell ref="M82:N85"/>
-    <mergeCell ref="M62:N65"/>
-    <mergeCell ref="M71:N76"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="P62:P65"/>
-    <mergeCell ref="Q62:Q65"/>
-    <mergeCell ref="Z66:AB66"/>
-    <mergeCell ref="Z67:AB67"/>
-    <mergeCell ref="Z68:AB68"/>
-    <mergeCell ref="Z69:AB69"/>
-    <mergeCell ref="Z70:AB70"/>
-    <mergeCell ref="Z71:AB71"/>
-    <mergeCell ref="Z72:AB72"/>
-    <mergeCell ref="C50:AG50"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="J62:J65"/>
-    <mergeCell ref="AY60:AY72"/>
-    <mergeCell ref="AX78:AY78"/>
-    <mergeCell ref="AY81:AY85"/>
-    <mergeCell ref="AY87:AY91"/>
-    <mergeCell ref="AQ78:AR81"/>
-    <mergeCell ref="AU71:AV71"/>
-    <mergeCell ref="AQ61:AR64"/>
-    <mergeCell ref="B57:D59"/>
-    <mergeCell ref="P57:Q59"/>
-    <mergeCell ref="Q71:Q76"/>
-    <mergeCell ref="Z78:AB78"/>
-    <mergeCell ref="Z79:AB79"/>
-    <mergeCell ref="Z80:AB80"/>
-    <mergeCell ref="Z81:AB81"/>
-    <mergeCell ref="Z82:AB82"/>
-    <mergeCell ref="Z73:AB73"/>
-    <mergeCell ref="Z74:AB74"/>
-    <mergeCell ref="Z75:AB75"/>
-    <mergeCell ref="Z76:AB76"/>
-    <mergeCell ref="Z77:AB77"/>
-    <mergeCell ref="Z88:AB88"/>
-    <mergeCell ref="Z89:AB89"/>
-    <mergeCell ref="Z90:AB90"/>
-    <mergeCell ref="K62:K65"/>
+    <mergeCell ref="AI114:AK114"/>
+    <mergeCell ref="Z93:AB93"/>
+    <mergeCell ref="R105:AG105"/>
+    <mergeCell ref="H94:H97"/>
+    <mergeCell ref="I94:I97"/>
+    <mergeCell ref="B95:D97"/>
+    <mergeCell ref="E95:G97"/>
+    <mergeCell ref="J95:K97"/>
+    <mergeCell ref="L95:M97"/>
+    <mergeCell ref="N95:O97"/>
+    <mergeCell ref="P95:Q97"/>
+    <mergeCell ref="R95:V97"/>
+    <mergeCell ref="W95:X97"/>
+    <mergeCell ref="Y95:Z97"/>
+    <mergeCell ref="AA95:AB97"/>
+    <mergeCell ref="AC95:AG97"/>
     <mergeCell ref="AI111:AK111"/>
     <mergeCell ref="AI112:AK112"/>
-    <mergeCell ref="AN60:AN72"/>
-    <mergeCell ref="AN81:AN85"/>
-    <mergeCell ref="AN87:AN91"/>
-    <mergeCell ref="AQ71:AR71"/>
-    <mergeCell ref="AN78:AO78"/>
-    <mergeCell ref="AI107:AK107"/>
-    <mergeCell ref="AI108:AK108"/>
-    <mergeCell ref="AI109:AK109"/>
-    <mergeCell ref="AI110:AK110"/>
-    <mergeCell ref="AI102:AK102"/>
-    <mergeCell ref="AI103:AK103"/>
-    <mergeCell ref="AI104:AK104"/>
-    <mergeCell ref="AI105:AK105"/>
-    <mergeCell ref="AI106:AK106"/>
-    <mergeCell ref="AL106:AO106"/>
-    <mergeCell ref="AL107:AO107"/>
-    <mergeCell ref="AI100:AK100"/>
-    <mergeCell ref="AI101:AK101"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>